<commit_message>
Se agrego el campo apellidos a la tabla de equivalencia del Modulo Gestionar Usuario
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB1E3A8-293F-4DFC-BE80-0E502619D760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49C9D30-14A3-49D0-8D76-2F27CCB3BC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -146,13 +146,96 @@
   </si>
   <si>
     <t>CENV&lt;03&gt;</t>
+  </si>
+  <si>
+    <t>Apellidos</t>
+  </si>
+  <si>
+    <t>Lógico</t>
+  </si>
+  <si>
+    <t>Apellidos= caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <t>CEV&lt;02&gt;</t>
+  </si>
+  <si>
+    <t>Apellidos!= caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;04&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>1 &lt; Apellidos&lt;= 50</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;03&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Apellidos&lt;= 1</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;05&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Apellidos&gt; 50</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;06&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -208,6 +291,12 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF993300"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -412,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -514,16 +603,31 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -531,19 +635,19 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -829,7 +933,7 @@
   <dimension ref="B1:P1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -848,14 +952,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="35" t="s">
+      <c r="E3" s="41"/>
+      <c r="F3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="41"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -878,52 +982,99 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="35" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="44" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="36" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="44" t="s">
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="44" t="s">
+      <c r="G7" s="36" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="43"/>
+      <c r="C9" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="50" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -939,9 +1090,9 @@
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="37"/>
+      <c r="L22" s="39"/>
       <c r="M22" s="38"/>
-      <c r="N22" s="37"/>
+      <c r="N22" s="39"/>
       <c r="O22" s="38"/>
       <c r="P22" s="4"/>
     </row>
@@ -962,7 +1113,7 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="39"/>
+      <c r="O24" s="37"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -982,7 +1133,7 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="39"/>
+      <c r="O26" s="37"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1002,7 +1153,7 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="39"/>
+      <c r="O28" s="37"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2070,18 +2221,22 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
+  <mergeCells count="15">
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="E5:E7"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2111,20 +2266,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="45" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="36"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -2154,11 +2309,11 @@
       <c r="I3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="42"/>
-      <c r="L3" s="36"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="41"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">

</xml_diff>

<commit_message>
Se agrego el campo Nombres a la tabla de equivalencia del Modulo Gestionar Usuario
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49C9D30-14A3-49D0-8D76-2F27CCB3BC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12497BF-D175-412D-8DF6-EB18F20658E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -219,6 +219,94 @@
   <si>
     <r>
       <t>CENV&lt;06&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Nombres</t>
+  </si>
+  <si>
+    <t>Nombres= caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;04&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Nombres!= caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;07&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>1 &lt; Nombres&lt;= 50</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;05&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Nombres&lt;= 1</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;08&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Nombres&gt; 50</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;09&gt;</t>
     </r>
     <r>
       <rPr>
@@ -609,6 +697,34 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
@@ -616,39 +732,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -933,7 +1021,7 @@
   <dimension ref="B1:P1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -952,14 +1040,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="41"/>
-      <c r="F3" s="40" t="s">
+      <c r="E3" s="46"/>
+      <c r="F3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="41"/>
+      <c r="G3" s="46"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -982,16 +1070,16 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="40" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="35" t="s">
@@ -1002,10 +1090,10 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
       <c r="F6" s="36" t="s">
         <v>36</v>
       </c>
@@ -1014,10 +1102,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="36" t="s">
         <v>38</v>
       </c>
@@ -1026,58 +1114,105 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="49" t="s">
+      <c r="G8" s="38" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="43"/>
-      <c r="C9" s="42" t="s">
+      <c r="B9" s="41"/>
+      <c r="C9" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="50" t="s">
+      <c r="G9" s="39" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="50" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="50" t="s">
+      <c r="G10" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="41"/>
+      <c r="C12" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="14" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1090,10 +1225,10 @@
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="38"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="48"/>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1113,7 +1248,7 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="37"/>
+      <c r="O24" s="47"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1123,7 +1258,7 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="38"/>
+      <c r="O25" s="48"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1133,7 +1268,7 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="37"/>
+      <c r="O26" s="47"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1143,7 +1278,7 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="38"/>
+      <c r="O27" s="48"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1153,7 +1288,7 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="37"/>
+      <c r="O28" s="47"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1163,7 +1298,7 @@
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="38"/>
+      <c r="O29" s="48"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2221,22 +2356,26 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="19">
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2266,20 +2405,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="41"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="46"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -2309,11 +2448,11 @@
       <c r="I3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="46" t="s">
+      <c r="J3" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="47"/>
-      <c r="L3" s="41"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="46"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">

</xml_diff>

<commit_message>
Se agrego el campo Urbanizacion a la tabla de equivalencias del Modulo Gestionar Usuario
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12497BF-D175-412D-8DF6-EB18F20658E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D0449B-09F5-4E19-9408-0CC34E37E46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -318,12 +318,106 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
+  <si>
+    <t>Urbanización</t>
+  </si>
+  <si>
+    <t>Urbanización= caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;06&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Urbanización!= caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;10&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>1 &lt; Urbanización&lt;= 50</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;07&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Urbanización&lt;= 1</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;11&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Urbanización&gt; 50</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;12&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Urbanización= NULL</t>
+  </si>
+  <si>
+    <t>CEV&lt;08&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -387,6 +481,13 @@
       <color rgb="FF993300"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -589,7 +690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -721,10 +822,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
@@ -732,11 +829,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,7 +1125,7 @@
   <dimension ref="B1:P1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1040,14 +1144,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="45" t="s">
+      <c r="E3" s="49"/>
+      <c r="F3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="46"/>
+      <c r="G3" s="49"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1213,25 +1317,85 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="41"/>
+      <c r="C15" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="41"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="42"/>
+      <c r="C17" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+    </row>
+    <row r="18" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="48"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="46"/>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -1241,67 +1405,67 @@
       <c r="O23" s="6"/>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="47"/>
+      <c r="O24" s="45"/>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="48"/>
+      <c r="O25" s="46"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="47"/>
+      <c r="O26" s="45"/>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="48"/>
+      <c r="O27" s="46"/>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="47"/>
+      <c r="O28" s="45"/>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="48"/>
+      <c r="O29" s="46"/>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -1311,7 +1475,7 @@
       <c r="O30" s="7"/>
       <c r="P30" s="4"/>
     </row>
-    <row r="31" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -1321,7 +1485,7 @@
       <c r="O31" s="7"/>
       <c r="P31" s="4"/>
     </row>
-    <row r="32" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
@@ -2356,17 +2520,12 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="F3:G3"/>
+  <mergeCells count="23">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="D5:D7"/>
@@ -2375,7 +2534,16 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="O24:O25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2408,8 +2576,8 @@
       <c r="A1" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D2" s="51" t="s">
@@ -2418,7 +2586,7 @@
       <c r="E2" s="52"/>
       <c r="F2" s="52"/>
       <c r="G2" s="52"/>
-      <c r="H2" s="46"/>
+      <c r="H2" s="49"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -2452,7 +2620,7 @@
         <v>17</v>
       </c>
       <c r="K3" s="52"/>
-      <c r="L3" s="46"/>
+      <c r="L3" s="49"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">

</xml_diff>

<commit_message>
Se añadio el campo Manzana a la Tabla de Equivalencias del Modulo Gestionar Usuario
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D0449B-09F5-4E19-9408-0CC34E37E46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1BFFD3-698F-4C61-9EAE-8FD23D53653A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -411,6 +411,83 @@
   </si>
   <si>
     <t>CEV&lt;08&gt;</t>
+  </si>
+  <si>
+    <t>Manzana</t>
+  </si>
+  <si>
+    <t>Manzana= caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;09&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Manzana!= caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;13&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Manzana&lt;=1</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;10&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Manzana&gt; 1</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;14&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Manzana= NULL</t>
+  </si>
+  <si>
+    <t>CEV&lt;11&gt;</t>
   </si>
 </sst>
 </file>
@@ -807,6 +884,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -829,18 +913,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1125,7 +1202,7 @@
   <dimension ref="B1:P1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B18" sqref="B18:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1144,14 +1221,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="48" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="49"/>
+      <c r="G3" s="42"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1174,16 +1251,16 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="43" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="35" t="s">
@@ -1194,10 +1271,10 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
       <c r="F6" s="36" t="s">
         <v>36</v>
       </c>
@@ -1206,10 +1283,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="36" t="s">
         <v>38</v>
       </c>
@@ -1218,7 +1295,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="43" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="37" t="s">
@@ -1238,14 +1315,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
-      <c r="C9" s="40" t="s">
+      <c r="B9" s="44"/>
+      <c r="C9" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="46" t="s">
         <v>48</v>
       </c>
       <c r="F9" s="39" t="s">
@@ -1256,10 +1333,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="39" t="s">
         <v>51</v>
       </c>
@@ -1268,7 +1345,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="43" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="37" t="s">
@@ -1288,14 +1365,14 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="41"/>
-      <c r="C12" s="40" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="46" t="s">
         <v>59</v>
       </c>
       <c r="F12" s="39" t="s">
@@ -1306,10 +1383,10 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
       <c r="F13" s="39" t="s">
         <v>62</v>
       </c>
@@ -1318,7 +1395,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="43" t="s">
         <v>64</v>
       </c>
       <c r="C14" s="37" t="s">
@@ -1338,14 +1415,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="41"/>
-      <c r="C15" s="40" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="46" t="s">
         <v>70</v>
       </c>
       <c r="F15" s="39" t="s">
@@ -1356,10 +1433,10 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
       <c r="F16" s="39" t="s">
         <v>73</v>
       </c>
@@ -1368,7 +1445,7 @@
       </c>
     </row>
     <row r="17" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="42"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="36" t="s">
         <v>41</v>
       </c>
@@ -1378,21 +1455,77 @@
       <c r="E17" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-    </row>
-    <row r="18" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+    </row>
+    <row r="18" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="44"/>
+      <c r="C19" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="44"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+    </row>
+    <row r="21" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="45"/>
+      <c r="C21" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+    </row>
     <row r="22" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="46"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="46"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="49"/>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1412,7 +1545,7 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="45"/>
+      <c r="O24" s="48"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1422,7 +1555,7 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="46"/>
+      <c r="O25" s="49"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1432,7 +1565,7 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="45"/>
+      <c r="O26" s="48"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1442,7 +1575,7 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="46"/>
+      <c r="O27" s="49"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1452,7 +1585,7 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="45"/>
+      <c r="O28" s="48"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1462,7 +1595,7 @@
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="46"/>
+      <c r="O29" s="49"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2520,7 +2653,20 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="29">
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C15:C16"/>
@@ -2534,16 +2680,9 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="O24:O25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2573,20 +2712,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="49"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -2616,11 +2755,11 @@
       <c r="I3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="51" t="s">
+      <c r="J3" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="52"/>
-      <c r="L3" s="49"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="42"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">

</xml_diff>

<commit_message>
Se añadio el campo Lote a la Tabla de Equivalencias del Modulo Gestionar Usuario
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1BFFD3-698F-4C61-9EAE-8FD23D53653A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDB3472-C410-43F5-BB79-7BA9D9CE4C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="98">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -488,6 +488,80 @@
   </si>
   <si>
     <t>CEV&lt;11&gt;</t>
+  </si>
+  <si>
+    <t>Lote</t>
+  </si>
+  <si>
+    <t>0&lt;Lote&lt;=99</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;12&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Lote!= caracteres numéricos</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;15&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Lote&lt;= 0</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;16&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Lote&gt; 99</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;17&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>CEV&lt;13&gt;</t>
   </si>
 </sst>
 </file>
@@ -767,7 +841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -887,37 +961,40 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1202,7 +1279,7 @@
   <dimension ref="B1:P1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:G21"/>
+      <selection activeCell="B22" sqref="B22:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1221,14 +1298,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="41" t="s">
+      <c r="E3" s="50"/>
+      <c r="F3" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="42"/>
+      <c r="G3" s="50"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1251,16 +1328,16 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="45" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="35" t="s">
@@ -1271,10 +1348,10 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
       <c r="F6" s="36" t="s">
         <v>36</v>
       </c>
@@ -1283,10 +1360,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="36" t="s">
         <v>38</v>
       </c>
@@ -1295,7 +1372,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="45" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="37" t="s">
@@ -1315,14 +1392,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="44"/>
-      <c r="C9" s="43" t="s">
+      <c r="B9" s="46"/>
+      <c r="C9" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="41" t="s">
         <v>48</v>
       </c>
       <c r="F9" s="39" t="s">
@@ -1333,10 +1410,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="39" t="s">
         <v>51</v>
       </c>
@@ -1345,7 +1422,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="45" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="37" t="s">
@@ -1365,14 +1442,14 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="44"/>
-      <c r="C12" s="43" t="s">
+      <c r="B12" s="46"/>
+      <c r="C12" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="41" t="s">
         <v>59</v>
       </c>
       <c r="F12" s="39" t="s">
@@ -1383,10 +1460,10 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="39" t="s">
         <v>62</v>
       </c>
@@ -1395,7 +1472,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="45" t="s">
         <v>64</v>
       </c>
       <c r="C14" s="37" t="s">
@@ -1415,14 +1492,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="44"/>
-      <c r="C15" s="43" t="s">
+      <c r="B15" s="46"/>
+      <c r="C15" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="46" t="s">
+      <c r="E15" s="41" t="s">
         <v>70</v>
       </c>
       <c r="F15" s="39" t="s">
@@ -1433,10 +1510,10 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="39" t="s">
         <v>73</v>
       </c>
@@ -1445,7 +1522,7 @@
       </c>
     </row>
     <row r="17" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="45"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="36" t="s">
         <v>41</v>
       </c>
@@ -1459,7 +1536,7 @@
       <c r="G17" s="40"/>
     </row>
     <row r="18" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="45" t="s">
         <v>77</v>
       </c>
       <c r="C18" s="37" t="s">
@@ -1479,33 +1556,33 @@
       </c>
     </row>
     <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="44"/>
-      <c r="C19" s="43" t="s">
+      <c r="B19" s="46"/>
+      <c r="C19" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="46" t="s">
+      <c r="F19" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="46" t="s">
+      <c r="G19" s="41" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
     </row>
     <row r="21" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="45"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="36" t="s">
         <v>41</v>
       </c>
@@ -1518,17 +1595,45 @@
       <c r="F21" s="40"/>
       <c r="G21" s="40"/>
     </row>
-    <row r="22" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>92</v>
+      </c>
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="49"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="44"/>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" s="39" t="s">
+        <v>94</v>
+      </c>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -1538,24 +1643,46 @@
       <c r="O23" s="6"/>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="46"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" s="39" t="s">
+        <v>96</v>
+      </c>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="48"/>
+      <c r="O24" s="43"/>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="47"/>
+      <c r="C25" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="49"/>
+      <c r="O25" s="44"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1565,7 +1692,7 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="48"/>
+      <c r="O26" s="43"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1575,7 +1702,7 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="49"/>
+      <c r="O27" s="44"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1585,7 +1712,7 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="48"/>
+      <c r="O28" s="43"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1595,7 +1722,7 @@
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="49"/>
+      <c r="O29" s="44"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2653,20 +2780,7 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="F3:G3"/>
+  <mergeCells count="33">
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C15:C16"/>
@@ -2683,6 +2797,23 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2715,8 +2846,8 @@
       <c r="A1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D2" s="52" t="s">
@@ -2725,7 +2856,7 @@
       <c r="E2" s="53"/>
       <c r="F2" s="53"/>
       <c r="G2" s="53"/>
-      <c r="H2" s="42"/>
+      <c r="H2" s="50"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -2759,7 +2890,7 @@
         <v>17</v>
       </c>
       <c r="K3" s="53"/>
-      <c r="L3" s="42"/>
+      <c r="L3" s="50"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">

</xml_diff>

<commit_message>
Se añadio el campo Distrito a la Tabla de Equivalencias del Modulo Gestionar Usuario
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDB3472-C410-43F5-BB79-7BA9D9CE4C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115B08B6-7518-419C-92A1-BF5342FF646E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="110">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -562,6 +562,97 @@
   </si>
   <si>
     <t>CEV&lt;13&gt;</t>
+  </si>
+  <si>
+    <t>Distrito</t>
+  </si>
+  <si>
+    <t>Distrito= caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;14&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Distrito!= caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;18&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>1 &lt; Distrito&lt;= 50</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;15&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Distrito&lt;= 1</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;19&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Distrito&gt; 50</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;20&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>CEV&lt;16&gt;</t>
   </si>
 </sst>
 </file>
@@ -961,6 +1052,19 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -971,30 +1075,17 @@
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1279,7 +1370,7 @@
   <dimension ref="B1:P1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:G25"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1298,14 +1389,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="49" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="50"/>
+      <c r="G3" s="42"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1328,16 +1419,16 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="43" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="35" t="s">
@@ -1348,10 +1439,10 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
       <c r="F6" s="36" t="s">
         <v>36</v>
       </c>
@@ -1360,10 +1451,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="36" t="s">
         <v>38</v>
       </c>
@@ -1372,7 +1463,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="43" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="37" t="s">
@@ -1392,14 +1483,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46"/>
-      <c r="C9" s="45" t="s">
+      <c r="B9" s="44"/>
+      <c r="C9" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="46" t="s">
         <v>48</v>
       </c>
       <c r="F9" s="39" t="s">
@@ -1410,10 +1501,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="39" t="s">
         <v>51</v>
       </c>
@@ -1422,7 +1513,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="43" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="37" t="s">
@@ -1442,14 +1533,14 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46"/>
-      <c r="C12" s="45" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="41" t="s">
+      <c r="E12" s="46" t="s">
         <v>59</v>
       </c>
       <c r="F12" s="39" t="s">
@@ -1460,10 +1551,10 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
       <c r="F13" s="39" t="s">
         <v>62</v>
       </c>
@@ -1472,7 +1563,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="43" t="s">
         <v>64</v>
       </c>
       <c r="C14" s="37" t="s">
@@ -1492,14 +1583,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="46"/>
-      <c r="C15" s="45" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="41" t="s">
+      <c r="E15" s="46" t="s">
         <v>70</v>
       </c>
       <c r="F15" s="39" t="s">
@@ -1510,10 +1601,10 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="46"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
       <c r="F16" s="39" t="s">
         <v>73</v>
       </c>
@@ -1522,7 +1613,7 @@
       </c>
     </row>
     <row r="17" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="36" t="s">
         <v>41</v>
       </c>
@@ -1536,7 +1627,7 @@
       <c r="G17" s="40"/>
     </row>
     <row r="18" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="43" t="s">
         <v>77</v>
       </c>
       <c r="C18" s="37" t="s">
@@ -1556,33 +1647,33 @@
       </c>
     </row>
     <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="46"/>
-      <c r="C19" s="45" t="s">
+      <c r="B19" s="44"/>
+      <c r="C19" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="41" t="s">
+      <c r="D19" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="41" t="s">
+      <c r="E19" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="41" t="s">
+      <c r="F19" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="41" t="s">
+      <c r="G19" s="46" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="46"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
     </row>
     <row r="21" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="47"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="36" t="s">
         <v>41</v>
       </c>
@@ -1596,16 +1687,16 @@
       <c r="G21" s="40"/>
     </row>
     <row r="22" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="41" t="s">
+      <c r="D22" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="41" t="s">
+      <c r="E22" s="46" t="s">
         <v>90</v>
       </c>
       <c r="F22" s="38" t="s">
@@ -1617,17 +1708,17 @@
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="48"/>
-      <c r="O22" s="44"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="49"/>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
       <c r="F23" s="39" t="s">
         <v>93</v>
       </c>
@@ -1644,10 +1735,10 @@
       <c r="P23" s="4"/>
     </row>
     <row r="24" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
       <c r="F24" s="39" t="s">
         <v>95</v>
       </c>
@@ -1660,11 +1751,11 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="43"/>
+      <c r="O24" s="48"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="36" t="s">
         <v>41</v>
       </c>
@@ -1682,47 +1773,103 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="44"/>
+      <c r="O25" s="49"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="G26" s="38" t="s">
+        <v>102</v>
+      </c>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="43"/>
+      <c r="O26" s="48"/>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="44"/>
+      <c r="C27" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="G27" s="39" t="s">
+        <v>106</v>
+      </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="44"/>
+      <c r="O27" s="49"/>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="44"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" s="39" t="s">
+        <v>108</v>
+      </c>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="43"/>
+      <c r="O28" s="48"/>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="45"/>
+      <c r="C29" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="44"/>
+      <c r="O29" s="49"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2780,7 +2927,28 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="37">
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C15:C16"/>
@@ -2797,23 +2965,6 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2843,20 +2994,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="50"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -2886,11 +3037,11 @@
       <c r="I3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="J3" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="53"/>
-      <c r="L3" s="50"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="42"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">

</xml_diff>

<commit_message>
Se añadio el campo Provincia a la Tabla de Equivalencias del Modulo Gestionar Usuario
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115B08B6-7518-419C-92A1-BF5342FF646E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FC6CC0-1127-4FA5-AA0C-9EA2E1487FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="122">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -653,6 +653,97 @@
   </si>
   <si>
     <t>CEV&lt;16&gt;</t>
+  </si>
+  <si>
+    <t>Provincia</t>
+  </si>
+  <si>
+    <t>Provincia= caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;17&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Provincia!= caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;21&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>1 &lt; Provincia&lt;= 50</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;18&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Provincia&lt;= 1</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;22&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Provincia&gt; 50</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;23&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>CEV&lt;19&gt;</t>
   </si>
 </sst>
 </file>
@@ -1052,35 +1143,35 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1370,7 +1461,7 @@
   <dimension ref="B1:P1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="B30" sqref="B30:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1389,14 +1480,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="41" t="s">
+      <c r="E3" s="51"/>
+      <c r="F3" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="42"/>
+      <c r="G3" s="51"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1419,16 +1510,16 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="41" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="35" t="s">
@@ -1439,10 +1530,10 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
       <c r="F6" s="36" t="s">
         <v>36</v>
       </c>
@@ -1451,10 +1542,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
       <c r="F7" s="36" t="s">
         <v>38</v>
       </c>
@@ -1463,7 +1554,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="41" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="37" t="s">
@@ -1483,14 +1574,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="44"/>
-      <c r="C9" s="43" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="44" t="s">
         <v>48</v>
       </c>
       <c r="F9" s="39" t="s">
@@ -1501,10 +1592,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="39" t="s">
         <v>51</v>
       </c>
@@ -1513,7 +1604,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="41" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="37" t="s">
@@ -1533,14 +1624,14 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="44"/>
-      <c r="C12" s="43" t="s">
+      <c r="B12" s="42"/>
+      <c r="C12" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="44" t="s">
         <v>59</v>
       </c>
       <c r="F12" s="39" t="s">
@@ -1551,10 +1642,10 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="39" t="s">
         <v>62</v>
       </c>
@@ -1563,7 +1654,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="41" t="s">
         <v>64</v>
       </c>
       <c r="C14" s="37" t="s">
@@ -1583,14 +1674,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="44"/>
-      <c r="C15" s="43" t="s">
+      <c r="B15" s="42"/>
+      <c r="C15" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="46" t="s">
+      <c r="E15" s="44" t="s">
         <v>70</v>
       </c>
       <c r="F15" s="39" t="s">
@@ -1601,10 +1692,10 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
       <c r="F16" s="39" t="s">
         <v>73</v>
       </c>
@@ -1613,7 +1704,7 @@
       </c>
     </row>
     <row r="17" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="45"/>
+      <c r="B17" s="43"/>
       <c r="C17" s="36" t="s">
         <v>41</v>
       </c>
@@ -1627,7 +1718,7 @@
       <c r="G17" s="40"/>
     </row>
     <row r="18" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="41" t="s">
         <v>77</v>
       </c>
       <c r="C18" s="37" t="s">
@@ -1647,33 +1738,33 @@
       </c>
     </row>
     <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="44"/>
-      <c r="C19" s="43" t="s">
+      <c r="B19" s="42"/>
+      <c r="C19" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="46" t="s">
+      <c r="F19" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="46" t="s">
+      <c r="G19" s="44" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
     </row>
     <row r="21" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="45"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="36" t="s">
         <v>41</v>
       </c>
@@ -1687,16 +1778,16 @@
       <c r="G21" s="40"/>
     </row>
     <row r="22" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="46" t="s">
+      <c r="D22" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="46" t="s">
+      <c r="E22" s="44" t="s">
         <v>90</v>
       </c>
       <c r="F22" s="38" t="s">
@@ -1708,17 +1799,17 @@
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="47"/>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
       <c r="F23" s="39" t="s">
         <v>93</v>
       </c>
@@ -1735,10 +1826,10 @@
       <c r="P23" s="4"/>
     </row>
     <row r="24" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="44"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
       <c r="F24" s="39" t="s">
         <v>95</v>
       </c>
@@ -1751,11 +1842,11 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="48"/>
+      <c r="O24" s="46"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="45"/>
+      <c r="B25" s="43"/>
       <c r="C25" s="36" t="s">
         <v>41</v>
       </c>
@@ -1773,11 +1864,11 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="49"/>
+      <c r="O25" s="47"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="41" t="s">
         <v>98</v>
       </c>
       <c r="C26" s="37" t="s">
@@ -1801,18 +1892,18 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="48"/>
+      <c r="O26" s="46"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="44"/>
-      <c r="C27" s="43" t="s">
+      <c r="B27" s="42"/>
+      <c r="C27" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="46" t="s">
+      <c r="D27" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="E27" s="46" t="s">
+      <c r="E27" s="44" t="s">
         <v>104</v>
       </c>
       <c r="F27" s="39" t="s">
@@ -1827,14 +1918,14 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="49"/>
+      <c r="O27" s="47"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="44"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
       <c r="F28" s="39" t="s">
         <v>107</v>
       </c>
@@ -1847,11 +1938,11 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="48"/>
+      <c r="O28" s="46"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="45"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="36" t="s">
         <v>41</v>
       </c>
@@ -1869,10 +1960,28 @@
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="49"/>
+      <c r="O29" s="47"/>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="38" t="s">
+        <v>114</v>
+      </c>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -1882,7 +1991,23 @@
       <c r="O30" s="7"/>
       <c r="P30" s="4"/>
     </row>
-    <row r="31" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="42"/>
+      <c r="C31" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="G31" s="39" t="s">
+        <v>118</v>
+      </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -1892,7 +2017,17 @@
       <c r="O31" s="7"/>
       <c r="P31" s="4"/>
     </row>
-    <row r="32" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="42"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="G32" s="39" t="s">
+        <v>120</v>
+      </c>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
@@ -1902,7 +2037,19 @@
       <c r="O32" s="7"/>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="43"/>
+      <c r="C33" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -1912,7 +2059,7 @@
       <c r="O33" s="7"/>
       <c r="P33" s="4"/>
     </row>
-    <row r="34" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -1922,7 +2069,7 @@
       <c r="O34" s="7"/>
       <c r="P34" s="4"/>
     </row>
-    <row r="35" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -1932,7 +2079,7 @@
       <c r="O35" s="7"/>
       <c r="P35" s="4"/>
     </row>
-    <row r="36" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -1942,7 +2089,7 @@
       <c r="O36" s="7"/>
       <c r="P36" s="4"/>
     </row>
-    <row r="37" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
@@ -1952,7 +2099,7 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
     </row>
-    <row r="38" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
@@ -1962,16 +2109,16 @@
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
     </row>
-    <row r="39" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="9:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2927,28 +3074,11 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="F3:G3"/>
+  <mergeCells count="41">
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C15:C16"/>
@@ -2965,6 +3095,27 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E12:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2997,8 +3148,8 @@
       <c r="A1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D2" s="53" t="s">
@@ -3007,7 +3158,7 @@
       <c r="E2" s="54"/>
       <c r="F2" s="54"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="42"/>
+      <c r="H2" s="51"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -3041,7 +3192,7 @@
         <v>17</v>
       </c>
       <c r="K3" s="54"/>
-      <c r="L3" s="42"/>
+      <c r="L3" s="51"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">

</xml_diff>

<commit_message>
Se añadio el campo Nombre rol descripcion a la Tabla de Equivalencias del Modulo Gestionar Usuario
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FC6CC0-1127-4FA5-AA0C-9EA2E1487FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E89D32-80CE-47D8-BB8F-4B011CFB6548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="130">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -744,6 +744,74 @@
   </si>
   <si>
     <t>CEV&lt;19&gt;</t>
+  </si>
+  <si>
+    <t>Nombre rol descripcion</t>
+  </si>
+  <si>
+    <r>
+      <t>Miembro de un Conjunto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Nombre rol descripcion= Administrador</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;20&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Nombre rol descripcion = Empleado</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;21&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Nombre rol descripcion= NULL</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;22&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1023,7 +1091,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1158,25 +1226,34 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1461,7 +1538,7 @@
   <dimension ref="B1:P1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:G33"/>
+      <selection activeCell="E9" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1480,14 +1557,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="51"/>
-      <c r="F3" s="50" t="s">
+      <c r="E3" s="47"/>
+      <c r="F3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="47"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1799,17 +1876,17 @@
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="47"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="49"/>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="42"/>
       <c r="C23" s="42"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
       <c r="F23" s="39" t="s">
         <v>93</v>
       </c>
@@ -1842,7 +1919,7 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="46"/>
+      <c r="O24" s="48"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1864,7 +1941,7 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="47"/>
+      <c r="O25" s="49"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1892,7 +1969,7 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="46"/>
+      <c r="O26" s="48"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1918,7 +1995,7 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="47"/>
+      <c r="O27" s="49"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1938,7 +2015,7 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="46"/>
+      <c r="O28" s="48"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1960,7 +2037,7 @@
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="47"/>
+      <c r="O29" s="49"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2059,7 +2136,21 @@
       <c r="O33" s="7"/>
       <c r="P33" s="4"/>
     </row>
-    <row r="34" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -2069,7 +2160,17 @@
       <c r="O34" s="7"/>
       <c r="P34" s="4"/>
     </row>
-    <row r="35" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -2079,7 +2180,17 @@
       <c r="O35" s="7"/>
       <c r="P35" s="4"/>
     </row>
-    <row r="36" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -3074,7 +3185,36 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="45">
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="D31:D32"/>
@@ -3091,31 +3231,6 @@
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E12:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3148,8 +3263,8 @@
       <c r="A1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D2" s="53" t="s">
@@ -3158,7 +3273,7 @@
       <c r="E2" s="54"/>
       <c r="F2" s="54"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="51"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -3192,7 +3307,7 @@
         <v>17</v>
       </c>
       <c r="K3" s="54"/>
-      <c r="L3" s="51"/>
+      <c r="L3" s="47"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">

</xml_diff>

<commit_message>
Se añadio Los casos de Prueba CP1 y CP2 para entradas correctas sin errores para reportar
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E89D32-80CE-47D8-BB8F-4B011CFB6548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841C514E-D9B5-4544-A36A-E1981F7EA5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clases de equialencia Nuevo U" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="142">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -46,34 +46,13 @@
     <t>Código</t>
   </si>
   <si>
-    <t>AGREGAR USUARIO</t>
-  </si>
-  <si>
     <t>CONDICIONES DE ENTRADA</t>
   </si>
   <si>
     <t>Caso prueba</t>
   </si>
   <si>
-    <t xml:space="preserve">Escenario </t>
-  </si>
-  <si>
     <t>Clases de equivalencia</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>Contraseña</t>
-  </si>
-  <si>
-    <t>Tipo de Perfil</t>
-  </si>
-  <si>
-    <t>Foto</t>
   </si>
   <si>
     <t>Resultado esperado</t>
@@ -813,12 +792,69 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
+  <si>
+    <t>Nuevo Usuario</t>
+  </si>
+  <si>
+    <t>Escenario</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Registro Exitroso</t>
+  </si>
+  <si>
+    <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;06&gt;,CEV&lt;09&gt; , CEV&lt;12&gt; , CEV&lt;14&gt; , CEV&lt;17&gt; , CEV&lt;22&gt;</t>
+  </si>
+  <si>
+    <t>Araujo Bravo</t>
+  </si>
+  <si>
+    <t>Juan Alberto</t>
+  </si>
+  <si>
+    <t>Las lomas</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Comas</t>
+  </si>
+  <si>
+    <t>Lima</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Se Registra correctamente el Usuario</t>
+  </si>
+  <si>
+    <t>Se registra y se muestra el mensaje: "Usuario creado/a satisfactoriamente"</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;08&gt; ,CEV&lt;11&gt; ,CEV&lt;16&gt; , CEV&lt;14&gt; , CEV&lt;19&gt; , CEV&lt;21&gt;</t>
+  </si>
+  <si>
+    <t>Aliaga Froilan</t>
+  </si>
+  <si>
+    <t>Felipe</t>
+  </si>
+  <si>
+    <t>Empleado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -890,8 +926,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -908,12 +957,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDAEEF3"/>
-        <bgColor rgb="FFDAEEF3"/>
       </patternFill>
     </fill>
     <fill>
@@ -946,8 +989,20 @@
         <bgColor rgb="FF9FC5E8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEEF3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1001,17 +1056,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -1087,11 +1131,93 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1112,11 +1238,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1124,15 +1247,12 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1181,35 +1301,41 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1217,19 +1343,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1237,22 +1350,52 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1316,6 +1459,72 @@
         <a:xfrm>
           <a:off x="7810500" y="0"/>
           <a:ext cx="8162925" cy="6173268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>400050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>438150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AD87E7B-5B38-E255-A332-F46A9084ED77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="17078325" y="752475"/>
+          <a:ext cx="2238375" cy="447675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1537,7 +1746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
@@ -1587,311 +1796,311 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+    </row>
+    <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="G7" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="41" t="s">
+    </row>
+    <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="C8" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="D8" s="32" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="36" t="s">
+      <c r="E8" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="F8" s="32" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="36" t="s">
+      <c r="G8" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="36" t="s">
+    </row>
+    <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="41"/>
+      <c r="C9" s="40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="41" t="s">
+      <c r="D9" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="E9" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="F9" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="G9" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="38" t="s">
+    </row>
+    <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G10" s="33" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="42"/>
-      <c r="C9" s="41" t="s">
+    <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="C11" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E11" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F11" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G11" s="32" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="39" t="s">
+    <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="41"/>
+      <c r="C12" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="E12" s="38" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="41" t="s">
+      <c r="F12" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="38" t="s">
+      <c r="G12" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="38" t="s">
+    </row>
+    <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="38" t="s">
+      <c r="G13" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="38" t="s">
+    </row>
+    <row r="14" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="40" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="42"/>
-      <c r="C12" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="44" t="s">
+      <c r="C14" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="44" t="s">
+      <c r="E14" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="F14" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G14" s="32" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="39" t="s">
+    <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="41"/>
+      <c r="C15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="39" t="s">
+      <c r="E15" s="38" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="41" t="s">
+      <c r="F15" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="38" t="s">
+      <c r="G15" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="38" t="s">
+    </row>
+    <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="41"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="G16" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="38" t="s">
+    </row>
+    <row r="17" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="42"/>
+      <c r="C17" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="33" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="42"/>
-      <c r="C15" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="44" t="s">
+      <c r="E17" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="44" t="s">
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+    </row>
+    <row r="18" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="39" t="s">
+      <c r="C18" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="39" t="s">
+      <c r="E18" s="32" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="39" t="s">
+      <c r="F18" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="G18" s="32" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="43"/>
-      <c r="C17" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="39" t="s">
+    <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="41"/>
+      <c r="C19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E19" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-    </row>
-    <row r="18" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="41" t="s">
+      <c r="F19" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="38" t="s">
+      <c r="G19" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="38" t="s">
+    </row>
+    <row r="20" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="41"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+    </row>
+    <row r="21" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="42"/>
+      <c r="C21" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="F18" s="38" t="s">
+      <c r="E21" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="38" t="s">
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+    </row>
+    <row r="22" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="40" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="42"/>
-      <c r="C19" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="44" t="s">
+      <c r="C22" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="44" t="s">
+      <c r="E22" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="44" t="s">
+      <c r="F22" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="44" t="s">
+      <c r="G22" s="32" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="42"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-    </row>
-    <row r="21" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="43"/>
-      <c r="C21" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-    </row>
-    <row r="22" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="F22" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="G22" s="38" t="s">
-        <v>92</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="49"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="44"/>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" s="39" t="s">
-        <v>94</v>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>87</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -1903,15 +2112,15 @@
       <c r="P23" s="4"/>
     </row>
     <row r="24" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="G24" s="39" t="s">
-        <v>96</v>
+      <c r="B24" s="41"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>89</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -1919,49 +2128,49 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="48"/>
+      <c r="O24" s="43"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="43"/>
-      <c r="C25" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="49"/>
+      <c r="O25" s="44"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="E26" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="F26" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="G26" s="38" t="s">
-        <v>102</v>
+      <c r="B26" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>95</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
@@ -1969,25 +2178,25 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="48"/>
+      <c r="O26" s="43"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="42"/>
-      <c r="C27" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="E27" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="F27" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="G27" s="39" t="s">
-        <v>106</v>
+      <c r="B27" s="41"/>
+      <c r="C27" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>99</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
@@ -1995,19 +2204,19 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="49"/>
+      <c r="O27" s="44"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="42"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="G28" s="39" t="s">
-        <v>108</v>
+      <c r="B28" s="41"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="G28" s="33" t="s">
+        <v>101</v>
       </c>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
@@ -2015,49 +2224,49 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="48"/>
+      <c r="O28" s="43"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="43"/>
-      <c r="C29" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="E29" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="49"/>
+      <c r="O29" s="44"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="E30" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="F30" s="38" t="s">
-        <v>113</v>
-      </c>
-      <c r="G30" s="38" t="s">
-        <v>114</v>
+      <c r="B30" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="G30" s="32" t="s">
+        <v>107</v>
       </c>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
@@ -2069,21 +2278,21 @@
       <c r="P30" s="4"/>
     </row>
     <row r="31" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="42"/>
-      <c r="C31" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="E31" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="F31" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="G31" s="39" t="s">
-        <v>118</v>
+      <c r="B31" s="41"/>
+      <c r="C31" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>111</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
@@ -2095,15 +2304,15 @@
       <c r="P31" s="4"/>
     </row>
     <row r="32" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="42"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="G32" s="39" t="s">
-        <v>120</v>
+      <c r="B32" s="41"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="G32" s="33" t="s">
+        <v>113</v>
       </c>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
@@ -2115,18 +2324,18 @@
       <c r="P32" s="4"/>
     </row>
     <row r="33" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="43"/>
-      <c r="C33" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -2137,20 +2346,20 @@
       <c r="P33" s="4"/>
     </row>
     <row r="34" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="D34" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="E34" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="F34" s="55"/>
-      <c r="G34" s="55"/>
+      <c r="B34" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -2161,16 +2370,16 @@
       <c r="P34" s="4"/>
     </row>
     <row r="35" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="E35" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -2181,16 +2390,16 @@
       <c r="P35" s="4"/>
     </row>
     <row r="36" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="E36" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -3186,19 +3395,18 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C12:C13"/>
@@ -3215,22 +3423,23 @@
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="F34:F36"/>
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="E31:E32"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3240,10 +3449,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L991"/>
+  <dimension ref="A1:S991"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3254,251 +3463,356 @@
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
-    <col min="10" max="28" width="10" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="10" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="28" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="53" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-    </row>
-    <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="53" t="s">
-        <v>7</v>
       </c>
       <c r="E2" s="54"/>
       <c r="F2" s="54"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="47"/>
-    </row>
-    <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+    </row>
+    <row r="3" spans="1:19" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="D3" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="M3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="N3" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="O3" s="54"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="R3" s="54"/>
+      <c r="S3" s="55"/>
+    </row>
+    <row r="4" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="B4" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="57">
+        <v>2</v>
+      </c>
+      <c r="E4" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="57" t="s">
+        <v>131</v>
+      </c>
+      <c r="I4" s="57">
         <v>12</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="J4" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="K4" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="L4" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="M4" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="N4" s="60" t="s">
+        <v>136</v>
+      </c>
+      <c r="O4" s="61"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="R4" s="61"/>
+      <c r="S4" s="62"/>
+    </row>
+    <row r="5" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="59">
+        <v>50</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="59" t="s">
+        <v>140</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="I5" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="J5" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="K5" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="L5" s="59" t="s">
+        <v>141</v>
+      </c>
+      <c r="M5" s="59" t="s">
+        <v>135</v>
+      </c>
+      <c r="N5" s="60" t="s">
+        <v>136</v>
+      </c>
+      <c r="O5" s="61"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="R5" s="61"/>
+      <c r="S5" s="62"/>
+    </row>
+    <row r="6" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+    </row>
+    <row r="7" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+    </row>
+    <row r="8" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="53" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="47"/>
-    </row>
-    <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-    </row>
-    <row r="5" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-    </row>
-    <row r="6" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-    </row>
-    <row r="7" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-    </row>
-    <row r="8" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-    </row>
-    <row r="9" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-    </row>
-    <row r="10" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-    </row>
-    <row r="11" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-    </row>
-    <row r="12" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-    </row>
-    <row r="13" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-    </row>
-    <row r="14" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-    </row>
-    <row r="15" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="32"/>
-    </row>
-    <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="26"/>
+    </row>
+    <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4475,12 +4789,18 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:S5"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="N3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas Numero incorrectas sin errores para reportar
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841C514E-D9B5-4544-A36A-E1981F7EA5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8198E1-FC07-4166-B9B9-251EACF13F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="168">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -849,12 +849,124 @@
   <si>
     <t>Empleado</t>
   </si>
+  <si>
+    <t>Registro con Número Incorrecto</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;01&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;06&gt;,CEV&lt;09&gt; , CEV&lt;12&gt; , CEV&lt;14&gt; , CEV&lt;17&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Komatsu</t>
+  </si>
+  <si>
+    <t>Tomu</t>
+  </si>
+  <si>
+    <t>Las Flores</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Carabarillo</t>
+  </si>
+  <si>
+    <t>No se permite el Registro</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "/" como número</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;02&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;06&gt;,CEV&lt;09&gt; , CEV&lt;12&gt; , CEV&lt;14&gt; , CEV&lt;17&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>López</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t>San Isidro</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Tambo</t>
+  </si>
+  <si>
+    <t>Huancayo</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "99,,,,," como número</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;03&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;06&gt;,CEV&lt;09&gt; , CEV&lt;12&gt; , CEV&lt;14&gt; , CEV&lt;17&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Pérez</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Villa Real</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Oyon</t>
+  </si>
+  <si>
+    <t>Callao</t>
+  </si>
+  <si>
+    <t>No se permite el Registro y se muestra el Mensaje: "Es obligado que Número en Usuario tenga valor"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -939,6 +1051,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -957,12 +1075,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB6D7A8"/>
-        <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
     <fill>
@@ -998,6 +1110,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDAEEF3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1217,7 +1335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1289,18 +1407,6 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1319,6 +1425,56 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1328,73 +1484,41 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1525,6 +1649,67 @@
         <a:xfrm>
           <a:off x="17078325" y="752475"/>
           <a:ext cx="2238375" cy="447675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>185057</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>513658</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E629D94E-935D-EA99-8E09-2FB479691ABA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16944975" y="3914776"/>
+          <a:ext cx="2613932" cy="332682"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1766,14 +1951,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="46" t="s">
+      <c r="E3" s="39"/>
+      <c r="F3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="47"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1808,10 +1993,10 @@
       <c r="E5" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="25" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1820,10 +2005,10 @@
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
       <c r="E6" s="41"/>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="26" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1832,10 +2017,10 @@
       <c r="C7" s="42"/>
       <c r="D7" s="42"/>
       <c r="E7" s="42"/>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="26" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1843,19 +2028,19 @@
       <c r="B8" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="G8" s="28" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1864,28 +2049,28 @@
       <c r="C9" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="29" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="42"/>
       <c r="C10" s="42"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="33" t="s">
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="29" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1893,19 +2078,19 @@
       <c r="B11" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="28" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1914,28 +2099,28 @@
       <c r="C12" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="29" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="33" t="s">
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="G13" s="29" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1943,19 +2128,19 @@
       <c r="B14" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="28" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1964,62 +2149,62 @@
       <c r="C15" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="29" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="41"/>
       <c r="C16" s="42"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="33" t="s">
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G16" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="42"/>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
     </row>
     <row r="18" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="28" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2028,40 +2213,40 @@
       <c r="C19" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="38" t="s">
+      <c r="F19" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="38" t="s">
+      <c r="G19" s="43" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="41"/>
       <c r="C20" s="42"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
     </row>
     <row r="21" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="42"/>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
     </row>
     <row r="22" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="40" t="s">
@@ -2070,36 +2255,36 @@
       <c r="C22" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="38" t="s">
+      <c r="E22" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="G22" s="28" t="s">
         <v>85</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="44"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="46"/>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="33" t="s">
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G23" s="33" t="s">
+      <c r="G23" s="29" t="s">
         <v>87</v>
       </c>
       <c r="I23" s="5"/>
@@ -2114,12 +2299,12 @@
     <row r="24" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="41"/>
       <c r="C24" s="42"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="33" t="s">
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="G24" s="33" t="s">
+      <c r="G24" s="29" t="s">
         <v>89</v>
       </c>
       <c r="I24" s="5"/>
@@ -2128,48 +2313,48 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="43"/>
+      <c r="O24" s="45"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="42"/>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="44"/>
+      <c r="O25" s="46"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="32" t="s">
+      <c r="E26" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="32" t="s">
+      <c r="F26" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="G26" s="32" t="s">
+      <c r="G26" s="28" t="s">
         <v>95</v>
       </c>
       <c r="I26" s="5"/>
@@ -2178,7 +2363,7 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="43"/>
+      <c r="O26" s="45"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2186,16 +2371,16 @@
       <c r="C27" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="G27" s="29" t="s">
         <v>99</v>
       </c>
       <c r="I27" s="5"/>
@@ -2204,18 +2389,18 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="44"/>
+      <c r="O27" s="46"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="41"/>
       <c r="C28" s="42"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="33" t="s">
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="G28" s="33" t="s">
+      <c r="G28" s="29" t="s">
         <v>101</v>
       </c>
       <c r="I28" s="5"/>
@@ -2224,48 +2409,48 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="43"/>
+      <c r="O28" s="45"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="42"/>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="E29" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="44"/>
+      <c r="O29" s="46"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="32" t="s">
+      <c r="D30" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="E30" s="32" t="s">
+      <c r="E30" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="F30" s="32" t="s">
+      <c r="F30" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="G30" s="32" t="s">
+      <c r="G30" s="28" t="s">
         <v>107</v>
       </c>
       <c r="I30" s="5"/>
@@ -2282,16 +2467,16 @@
       <c r="C31" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="38" t="s">
+      <c r="E31" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="33" t="s">
+      <c r="F31" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="G31" s="33" t="s">
+      <c r="G31" s="29" t="s">
         <v>111</v>
       </c>
       <c r="I31" s="5"/>
@@ -2306,12 +2491,12 @@
     <row r="32" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="41"/>
       <c r="C32" s="42"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="33" t="s">
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="G32" s="33" t="s">
+      <c r="G32" s="29" t="s">
         <v>113</v>
       </c>
       <c r="I32" s="5"/>
@@ -2325,17 +2510,17 @@
     </row>
     <row r="33" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="42"/>
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="33" t="s">
+      <c r="E33" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -2352,14 +2537,14 @@
       <c r="C34" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="D34" s="32" t="s">
+      <c r="D34" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="E34" s="32" t="s">
+      <c r="E34" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -2372,14 +2557,14 @@
     <row r="35" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="41"/>
       <c r="C35" s="41"/>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="E35" s="33" t="s">
+      <c r="E35" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -2392,14 +2577,14 @@
     <row r="36" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="42"/>
       <c r="C36" s="42"/>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="E36" s="33" t="s">
+      <c r="E36" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -3395,6 +3580,35 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="E27:E28"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C15:C16"/>
@@ -3411,35 +3625,6 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3452,7 +3637,7 @@
   <dimension ref="A1:S991"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3473,344 +3658,449 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="53" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
     </row>
     <row r="3" spans="1:19" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="J3" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="K3" s="52" t="s">
+      <c r="K3" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="L3" s="52" t="s">
+      <c r="L3" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="52" t="s">
+      <c r="M3" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="53" t="s">
+      <c r="N3" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="54"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="53" t="s">
+      <c r="O3" s="53"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="R3" s="54"/>
-      <c r="S3" s="55"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="54"/>
     </row>
     <row r="4" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="57">
+      <c r="D4" s="35">
         <v>2</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="57" t="s">
+      <c r="H4" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="I4" s="57">
+      <c r="I4" s="35">
         <v>12</v>
       </c>
-      <c r="J4" s="57" t="s">
+      <c r="J4" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="K4" s="57" t="s">
+      <c r="K4" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="L4" s="57" t="s">
+      <c r="L4" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="M4" s="57" t="s">
+      <c r="M4" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="N4" s="60" t="s">
+      <c r="N4" s="55" t="s">
         <v>136</v>
       </c>
-      <c r="O4" s="61"/>
-      <c r="P4" s="62"/>
-      <c r="Q4" s="60" t="s">
+      <c r="O4" s="56"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="55" t="s">
         <v>137</v>
       </c>
-      <c r="R4" s="61"/>
-      <c r="S4" s="62"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="57"/>
     </row>
     <row r="5" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="59">
+      <c r="D5" s="37">
         <v>50</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I5" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="K5" s="59" t="s">
+      <c r="K5" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="L5" s="59" t="s">
+      <c r="L5" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="M5" s="59" t="s">
+      <c r="M5" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="N5" s="60" t="s">
+      <c r="N5" s="55" t="s">
         <v>136</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="60" t="s">
+      <c r="O5" s="56"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="55" t="s">
         <v>137</v>
       </c>
-      <c r="R5" s="61"/>
-      <c r="S5" s="62"/>
+      <c r="R5" s="56"/>
+      <c r="S5" s="57"/>
     </row>
-    <row r="6" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
+      <c r="B6" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="H6" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="I6" s="60">
+        <v>5</v>
+      </c>
+      <c r="J6" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="K6" s="60" t="s">
+        <v>133</v>
+      </c>
+      <c r="L6" s="60" t="s">
+        <v>134</v>
+      </c>
+      <c r="M6" s="60" t="s">
+        <v>150</v>
+      </c>
+      <c r="N6" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="O6" s="56"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="55" t="s">
+        <v>137</v>
+      </c>
+      <c r="R6" s="56"/>
+      <c r="S6" s="57"/>
     </row>
-    <row r="7" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
+      <c r="B7" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="61" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="62">
+        <v>9.9999999999999901E+36</v>
+      </c>
+      <c r="E7" s="62" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" s="62" t="s">
+        <v>154</v>
+      </c>
+      <c r="G7" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="H7" s="62" t="s">
+        <v>156</v>
+      </c>
+      <c r="I7" s="62">
+        <v>3</v>
+      </c>
+      <c r="J7" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="K7" s="62" t="s">
+        <v>158</v>
+      </c>
+      <c r="L7" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="M7" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="N7" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="O7" s="56"/>
+      <c r="P7" s="57"/>
+      <c r="Q7" s="55" t="s">
+        <v>137</v>
+      </c>
+      <c r="R7" s="56"/>
+      <c r="S7" s="57"/>
     </row>
-    <row r="8" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="B8" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="62">
+        <v>0</v>
+      </c>
+      <c r="E8" s="62" t="s">
+        <v>161</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="G8" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="H8" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="I8" s="62">
+        <v>5</v>
+      </c>
+      <c r="J8" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="K8" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="L8" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="M8" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="N8" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="O8" s="56"/>
+      <c r="P8" s="57"/>
+      <c r="Q8" s="55" t="s">
+        <v>137</v>
+      </c>
+      <c r="R8" s="56"/>
+      <c r="S8" s="57"/>
     </row>
     <row r="9" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
     </row>
     <row r="10" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="22"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="18"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="26"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="22"/>
     </row>
     <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4789,15 +5079,21 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="14">
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="N3:P3"/>
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="N5:P5"/>
     <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="N3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas Apellidos incorrectas se reporta errores en el CP6 y CP7
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8198E1-FC07-4166-B9B9-251EACF13F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5737681-6AE5-4365-8EB9-C975C9640599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="192">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -961,12 +961,144 @@
   <si>
     <t>No se permite el Registro y se muestra el Mensaje: "Es obligado que Número en Usuario tenga valor"</t>
   </si>
+  <si>
+    <t>Registro con Apellidos Incorrecto</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;04&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;04&gt;,CEV&lt;06&gt;,CEV&lt;09&gt; , CEV&lt;12&gt; , CEV&lt;14&gt; , CEV&lt;17&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Los Pinos</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Barranca</t>
+  </si>
+  <si>
+    <t>Juliaca</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir números y carácteres no alfanuméricos como Apellidos</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;05&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;04&gt;,CEV&lt;06&gt;,CEV&lt;09&gt; , CEV&lt;12&gt; , CEV&lt;14&gt; , CEV&lt;17&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Santa Rosa</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Bolognesi</t>
+  </si>
+  <si>
+    <t>Huaraz</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir Apellidos de una letra o menos</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;06&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;04&gt;,CEV&lt;06&gt;,CEV&lt;09&gt; , CEV&lt;12&gt; , CEV&lt;14&gt; , CEV&lt;17&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>dfdsfdsfdsfdsfwdfwwerfwefdsfdsfweffewfwerweqrwqfwegfwegrethgtyrhrtyhrtyhythjtyjdtrerhrdfhrehrehrehrterehrde</t>
+  </si>
+  <si>
+    <t>Mia</t>
+  </si>
+  <si>
+    <t>El Bosque</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Huaylas</t>
+  </si>
+  <si>
+    <t>Chachapoyas</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "dfdsfdsfdsfd,,,,," como Apellidos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1057,8 +1189,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1075,12 +1214,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB4A7D6"/>
-        <bgColor rgb="FFB4A7D6"/>
       </patternFill>
     </fill>
     <fill>
@@ -1116,6 +1249,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB6D7A8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4A7D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1335,7 +1480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1395,18 +1540,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1428,43 +1561,70 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1475,24 +1635,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1503,22 +1645,34 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1951,14 +2105,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="38" t="s">
+      <c r="E3" s="49"/>
+      <c r="F3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="39"/>
+      <c r="G3" s="49"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1981,310 +2135,310 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="21" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="26" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="22" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="26" t="s">
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
-      <c r="C9" s="40" t="s">
+      <c r="B9" s="43"/>
+      <c r="C9" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="29" t="s">
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="24" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="41"/>
-      <c r="C12" s="40" t="s">
+      <c r="B12" s="43"/>
+      <c r="C12" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="F12" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="29" t="s">
+      <c r="G12" s="25" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="29" t="s">
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="25" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="24" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="41"/>
-      <c r="C15" s="40" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="25" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="29" t="s">
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="25" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="42"/>
-      <c r="C17" s="26" t="s">
+      <c r="B17" s="44"/>
+      <c r="C17" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="G18" s="28" t="s">
+      <c r="G18" s="24" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="41"/>
-      <c r="C19" s="40" t="s">
+      <c r="B19" s="43"/>
+      <c r="C19" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="43" t="s">
+      <c r="F19" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="43" t="s">
+      <c r="G19" s="40" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="41"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
     </row>
     <row r="21" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="42"/>
-      <c r="C21" s="26" t="s">
+      <c r="B21" s="44"/>
+      <c r="C21" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="43" t="s">
+      <c r="D22" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="G22" s="28" t="s">
+      <c r="G22" s="24" t="s">
         <v>85</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="46"/>
-      <c r="N22" s="48"/>
-      <c r="O22" s="46"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="51"/>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="29" t="s">
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="G23" s="25" t="s">
         <v>87</v>
       </c>
       <c r="I23" s="5"/>
@@ -2297,14 +2451,14 @@
       <c r="P23" s="4"/>
     </row>
     <row r="24" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="41"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="29" t="s">
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="25" t="s">
         <v>89</v>
       </c>
       <c r="I24" s="5"/>
@@ -2313,48 +2467,48 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="45"/>
+      <c r="O24" s="50"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="42"/>
-      <c r="C25" s="26" t="s">
+      <c r="B25" s="44"/>
+      <c r="C25" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="46"/>
+      <c r="O25" s="51"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="G26" s="28" t="s">
+      <c r="G26" s="24" t="s">
         <v>95</v>
       </c>
       <c r="I26" s="5"/>
@@ -2363,24 +2517,24 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="45"/>
+      <c r="O26" s="50"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="41"/>
-      <c r="C27" s="40" t="s">
+      <c r="B27" s="43"/>
+      <c r="C27" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="43" t="s">
+      <c r="D27" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E27" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="29" t="s">
+      <c r="F27" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="G27" s="29" t="s">
+      <c r="G27" s="25" t="s">
         <v>99</v>
       </c>
       <c r="I27" s="5"/>
@@ -2389,18 +2543,18 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="46"/>
+      <c r="O27" s="51"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="41"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="29" t="s">
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="G28" s="29" t="s">
+      <c r="G28" s="25" t="s">
         <v>101</v>
       </c>
       <c r="I28" s="5"/>
@@ -2409,48 +2563,48 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="45"/>
+      <c r="O28" s="50"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="42"/>
-      <c r="C29" s="26" t="s">
+      <c r="B29" s="44"/>
+      <c r="C29" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="29" t="s">
+      <c r="E29" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="46"/>
+      <c r="O29" s="51"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="F30" s="28" t="s">
+      <c r="F30" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="G30" s="28" t="s">
+      <c r="G30" s="24" t="s">
         <v>107</v>
       </c>
       <c r="I30" s="5"/>
@@ -2463,20 +2617,20 @@
       <c r="P30" s="4"/>
     </row>
     <row r="31" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="41"/>
-      <c r="C31" s="40" t="s">
+      <c r="B31" s="43"/>
+      <c r="C31" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="43" t="s">
+      <c r="D31" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="43" t="s">
+      <c r="E31" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="29" t="s">
+      <c r="F31" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="G31" s="29" t="s">
+      <c r="G31" s="25" t="s">
         <v>111</v>
       </c>
       <c r="I31" s="5"/>
@@ -2489,14 +2643,14 @@
       <c r="P31" s="4"/>
     </row>
     <row r="32" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="41"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="29" t="s">
+      <c r="B32" s="43"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="G32" s="29" t="s">
+      <c r="G32" s="25" t="s">
         <v>113</v>
       </c>
       <c r="I32" s="5"/>
@@ -2509,18 +2663,18 @@
       <c r="P32" s="4"/>
     </row>
     <row r="33" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="42"/>
-      <c r="C33" s="26" t="s">
+      <c r="B33" s="44"/>
+      <c r="C33" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="29" t="s">
+      <c r="D33" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="29" t="s">
+      <c r="E33" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -2531,20 +2685,20 @@
       <c r="P33" s="4"/>
     </row>
     <row r="34" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="D34" s="28" t="s">
+      <c r="D34" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="E34" s="28" t="s">
+      <c r="E34" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -2555,16 +2709,16 @@
       <c r="P34" s="4"/>
     </row>
     <row r="35" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="29" t="s">
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="E35" s="29" t="s">
+      <c r="E35" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -2575,16 +2729,16 @@
       <c r="P35" s="4"/>
     </row>
     <row r="36" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="29" t="s">
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="E36" s="29" t="s">
+      <c r="E36" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -3580,35 +3734,6 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="E27:E28"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C15:C16"/>
@@ -3625,6 +3750,35 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3636,8 +3790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S991"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3658,449 +3812,554 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="52" t="s">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
     </row>
     <row r="3" spans="1:19" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="L3" s="33" t="s">
+      <c r="L3" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="33" t="s">
+      <c r="M3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="52" t="s">
+      <c r="N3" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="53"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="52" t="s">
+      <c r="O3" s="59"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="R3" s="53"/>
-      <c r="S3" s="54"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="60"/>
     </row>
     <row r="4" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="31">
         <v>2</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="31">
         <v>12</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="J4" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="K4" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="L4" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="M4" s="35" t="s">
+      <c r="M4" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="N4" s="55" t="s">
+      <c r="N4" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="O4" s="56"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="55" t="s">
+      <c r="O4" s="55"/>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="R4" s="56"/>
-      <c r="S4" s="57"/>
+      <c r="R4" s="55"/>
+      <c r="S4" s="56"/>
     </row>
     <row r="5" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="33">
         <v>50</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="I5" s="37" t="s">
+      <c r="I5" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="K5" s="37" t="s">
+      <c r="K5" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="L5" s="37" t="s">
+      <c r="L5" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="M5" s="37" t="s">
+      <c r="M5" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="N5" s="55" t="s">
+      <c r="N5" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="O5" s="56"/>
-      <c r="P5" s="57"/>
-      <c r="Q5" s="55" t="s">
+      <c r="O5" s="55"/>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="R5" s="56"/>
-      <c r="S5" s="57"/>
+      <c r="R5" s="55"/>
+      <c r="S5" s="56"/>
     </row>
     <row r="6" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="F6" s="60" t="s">
+      <c r="F6" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="G6" s="60" t="s">
+      <c r="G6" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="H6" s="60" t="s">
+      <c r="H6" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="I6" s="60">
+      <c r="I6" s="35">
         <v>5</v>
       </c>
-      <c r="J6" s="60" t="s">
+      <c r="J6" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="K6" s="60" t="s">
+      <c r="K6" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="L6" s="60" t="s">
+      <c r="L6" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="M6" s="60" t="s">
+      <c r="M6" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="N6" s="55" t="s">
+      <c r="N6" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="O6" s="56"/>
-      <c r="P6" s="57"/>
-      <c r="Q6" s="55" t="s">
+      <c r="O6" s="55"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="R6" s="56"/>
-      <c r="S6" s="57"/>
+      <c r="R6" s="55"/>
+      <c r="S6" s="56"/>
     </row>
     <row r="7" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="D7" s="62">
+      <c r="D7" s="37">
         <v>9.9999999999999901E+36</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="F7" s="62" t="s">
+      <c r="F7" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="G7" s="62" t="s">
+      <c r="G7" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="H7" s="62" t="s">
+      <c r="H7" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="I7" s="62">
+      <c r="I7" s="37">
         <v>3</v>
       </c>
-      <c r="J7" s="62" t="s">
+      <c r="J7" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="K7" s="62" t="s">
+      <c r="K7" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="L7" s="62" t="s">
+      <c r="L7" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="M7" s="62" t="s">
+      <c r="M7" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="N7" s="55" t="s">
+      <c r="N7" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="O7" s="56"/>
-      <c r="P7" s="57"/>
-      <c r="Q7" s="55" t="s">
+      <c r="O7" s="55"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="R7" s="56"/>
-      <c r="S7" s="57"/>
+      <c r="R7" s="55"/>
+      <c r="S7" s="56"/>
     </row>
     <row r="8" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="D8" s="62">
+      <c r="D8" s="37">
         <v>0</v>
       </c>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="F8" s="62" t="s">
+      <c r="F8" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="G8" s="62" t="s">
+      <c r="G8" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="H8" s="62" t="s">
+      <c r="H8" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="I8" s="62">
+      <c r="I8" s="37">
         <v>5</v>
       </c>
-      <c r="J8" s="62" t="s">
+      <c r="J8" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="K8" s="62" t="s">
+      <c r="K8" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L8" s="62" t="s">
+      <c r="L8" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="M8" s="62" t="s">
+      <c r="M8" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="N8" s="55" t="s">
+      <c r="N8" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="O8" s="56"/>
-      <c r="P8" s="57"/>
-      <c r="Q8" s="55" t="s">
+      <c r="O8" s="55"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="R8" s="56"/>
-      <c r="S8" s="57"/>
+      <c r="R8" s="55"/>
+      <c r="S8" s="56"/>
     </row>
-    <row r="9" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="B9" s="62" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="62" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" s="62">
+        <v>10</v>
+      </c>
+      <c r="E9" s="62">
+        <v>-54</v>
+      </c>
+      <c r="F9" s="62" t="s">
+        <v>170</v>
+      </c>
+      <c r="G9" s="62" t="s">
+        <v>171</v>
+      </c>
+      <c r="H9" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="I9" s="62">
+        <v>7</v>
+      </c>
+      <c r="J9" s="62" t="s">
+        <v>173</v>
+      </c>
+      <c r="K9" s="62" t="s">
+        <v>174</v>
+      </c>
+      <c r="L9" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="M9" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="N9" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="O9" s="66"/>
+      <c r="P9" s="67"/>
+      <c r="Q9" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="R9" s="55"/>
+      <c r="S9" s="56"/>
     </row>
-    <row r="10" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="B10" s="64" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="64" t="s">
+        <v>176</v>
+      </c>
+      <c r="D10" s="64">
+        <v>12</v>
+      </c>
+      <c r="E10" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="F10" s="64" t="s">
+        <v>178</v>
+      </c>
+      <c r="G10" s="64" t="s">
+        <v>179</v>
+      </c>
+      <c r="H10" s="64" t="s">
+        <v>180</v>
+      </c>
+      <c r="I10" s="64">
+        <v>8</v>
+      </c>
+      <c r="J10" s="64" t="s">
+        <v>181</v>
+      </c>
+      <c r="K10" s="64" t="s">
+        <v>182</v>
+      </c>
+      <c r="L10" s="64" t="s">
+        <v>134</v>
+      </c>
+      <c r="M10" s="64" t="s">
+        <v>150</v>
+      </c>
+      <c r="N10" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="O10" s="66"/>
+      <c r="P10" s="67"/>
+      <c r="Q10" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="R10" s="55"/>
+      <c r="S10" s="56"/>
     </row>
-    <row r="11" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
+      <c r="B11" s="64" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="64" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" s="64">
+        <v>51</v>
+      </c>
+      <c r="E11" s="64" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" s="64" t="s">
+        <v>186</v>
+      </c>
+      <c r="G11" s="64" t="s">
+        <v>187</v>
+      </c>
+      <c r="H11" s="64" t="s">
+        <v>188</v>
+      </c>
+      <c r="I11" s="64">
+        <v>10</v>
+      </c>
+      <c r="J11" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="K11" s="64" t="s">
+        <v>190</v>
+      </c>
+      <c r="L11" s="64" t="s">
+        <v>134</v>
+      </c>
+      <c r="M11" s="64" t="s">
+        <v>150</v>
+      </c>
+      <c r="N11" s="54" t="s">
+        <v>191</v>
+      </c>
+      <c r="O11" s="55"/>
+      <c r="P11" s="56"/>
+      <c r="Q11" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="R11" s="55"/>
+      <c r="S11" s="56"/>
     </row>
     <row r="12" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="18"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="14"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="22"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5079,21 +5338,27 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="20">
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
     <mergeCell ref="N6:P6"/>
     <mergeCell ref="Q6:S6"/>
     <mergeCell ref="N7:P7"/>
     <mergeCell ref="Q7:S7"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="Q5:S5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas Nombres incorrectas se reporta errores en el CP9 y CP10
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5737681-6AE5-4365-8EB9-C975C9640599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD020C9D-584D-4FEA-8F83-FB657E5AE26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="212">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -1092,6 +1092,126 @@
   </si>
   <si>
     <t>No se permite el ingreso de "dfdsfdsfdsfd,,,,," como Apellidos</t>
+  </si>
+  <si>
+    <t>Registro con Nombres Incorrecto</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;07&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;06&gt;,CEV&lt;09&gt; , CEV&lt;12&gt; , CEV&lt;14&gt; , CEV&lt;17&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>González</t>
+  </si>
+  <si>
+    <t>*//</t>
+  </si>
+  <si>
+    <t>Las Acacias</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir números y carácteres no alfanuméricos como Nombres</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;08&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;06&gt;,CEV&lt;09&gt; , CEV&lt;12&gt; , CEV&lt;14&gt; , CEV&lt;17&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Fernández</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>La Floresta</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Camana</t>
+  </si>
+  <si>
+    <t>Arequipa</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir Nombres de una letra o menos</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;09&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;06&gt;,CEV&lt;09&gt; , CEV&lt;12&gt; , CEV&lt;14&gt; , CEV&lt;17&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Torres</t>
+  </si>
+  <si>
+    <t>fsdsgfdsgdsgdsfghdfsgdsfgdsgdsgdsgdssdgdsgsdgdsgddsgsdhsdrhggtedrgregdfxgfdxgerg</t>
+  </si>
+  <si>
+    <t>San Juan</t>
+  </si>
+  <si>
+    <t>La Union</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "fsdsgfdsgds,,,,," como Nombres</t>
   </si>
 </sst>
 </file>
@@ -1197,7 +1317,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1214,18 +1334,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6B8AF"/>
-        <bgColor rgb="FFE6B8AF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF9CB9C"/>
-        <bgColor rgb="FFF9CB9C"/>
       </patternFill>
     </fill>
     <fill>
@@ -1261,6 +1369,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6B8AF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1480,7 +1594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1501,9 +1615,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1516,30 +1627,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1561,12 +1648,42 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1579,22 +1696,17 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1603,14 +1715,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1621,20 +1731,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1644,14 +1743,23 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1664,15 +1772,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2105,14 +2204,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="48" t="s">
+      <c r="E3" s="36"/>
+      <c r="F3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="49"/>
+      <c r="G3" s="36"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -2135,72 +2234,72 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="22" t="s">
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="22" t="s">
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="15" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="43"/>
-      <c r="C9" s="42" t="s">
+      <c r="B9" s="38"/>
+      <c r="C9" s="37" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="40" t="s">
@@ -2209,48 +2308,48 @@
       <c r="E9" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="16" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="41"/>
       <c r="E10" s="41"/>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="15" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="43"/>
-      <c r="C12" s="42" t="s">
+      <c r="B12" s="38"/>
+      <c r="C12" s="37" t="s">
         <v>39</v>
       </c>
       <c r="D12" s="40" t="s">
@@ -2259,48 +2358,48 @@
       <c r="E12" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="16" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="41"/>
       <c r="E13" s="41"/>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="16" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="G14" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="43"/>
-      <c r="C15" s="42" t="s">
+      <c r="B15" s="38"/>
+      <c r="C15" s="37" t="s">
         <v>39</v>
       </c>
       <c r="D15" s="40" t="s">
@@ -2309,62 +2408,62 @@
       <c r="E15" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="43"/>
-      <c r="C16" s="44"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="41"/>
       <c r="E16" s="41"/>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="44"/>
-      <c r="C17" s="22" t="s">
+      <c r="B17" s="39"/>
+      <c r="C17" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
     </row>
     <row r="18" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="G18" s="24" t="s">
+      <c r="G18" s="15" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="43"/>
-      <c r="C19" s="42" t="s">
+      <c r="B19" s="38"/>
+      <c r="C19" s="37" t="s">
         <v>39</v>
       </c>
       <c r="D19" s="40" t="s">
@@ -2381,32 +2480,32 @@
       </c>
     </row>
     <row r="20" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="43"/>
-      <c r="C20" s="44"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
       <c r="D20" s="41"/>
       <c r="E20" s="41"/>
       <c r="F20" s="41"/>
       <c r="G20" s="41"/>
     </row>
     <row r="21" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="44"/>
-      <c r="C21" s="22" t="s">
+      <c r="B21" s="39"/>
+      <c r="C21" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E21" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
     </row>
     <row r="22" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="37" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="40" t="s">
@@ -2415,30 +2514,30 @@
       <c r="E22" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="F22" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="G22" s="15" t="s">
         <v>85</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="51"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="43"/>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="25" t="s">
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="G23" s="25" t="s">
+      <c r="G23" s="16" t="s">
         <v>87</v>
       </c>
       <c r="I23" s="5"/>
@@ -2451,14 +2550,14 @@
       <c r="P23" s="4"/>
     </row>
     <row r="24" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="43"/>
-      <c r="C24" s="44"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="39"/>
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="16" t="s">
         <v>89</v>
       </c>
       <c r="I24" s="5"/>
@@ -2467,48 +2566,48 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="50"/>
+      <c r="O24" s="42"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="44"/>
-      <c r="C25" s="22" t="s">
+      <c r="B25" s="39"/>
+      <c r="C25" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="51"/>
+      <c r="O25" s="43"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F26" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="G26" s="24" t="s">
+      <c r="G26" s="15" t="s">
         <v>95</v>
       </c>
       <c r="I26" s="5"/>
@@ -2517,12 +2616,12 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="50"/>
+      <c r="O26" s="42"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="43"/>
-      <c r="C27" s="42" t="s">
+      <c r="B27" s="38"/>
+      <c r="C27" s="37" t="s">
         <v>39</v>
       </c>
       <c r="D27" s="40" t="s">
@@ -2531,10 +2630,10 @@
       <c r="E27" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="25" t="s">
+      <c r="F27" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="G27" s="25" t="s">
+      <c r="G27" s="16" t="s">
         <v>99</v>
       </c>
       <c r="I27" s="5"/>
@@ -2543,18 +2642,18 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="51"/>
+      <c r="O27" s="43"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="43"/>
-      <c r="C28" s="44"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="39"/>
       <c r="D28" s="41"/>
       <c r="E28" s="41"/>
-      <c r="F28" s="25" t="s">
+      <c r="F28" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="G28" s="25" t="s">
+      <c r="G28" s="16" t="s">
         <v>101</v>
       </c>
       <c r="I28" s="5"/>
@@ -2563,48 +2662,48 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="50"/>
+      <c r="O28" s="42"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="44"/>
-      <c r="C29" s="22" t="s">
+      <c r="B29" s="39"/>
+      <c r="C29" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="51"/>
+      <c r="O29" s="43"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="F30" s="24" t="s">
+      <c r="F30" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="G30" s="24" t="s">
+      <c r="G30" s="15" t="s">
         <v>107</v>
       </c>
       <c r="I30" s="5"/>
@@ -2617,8 +2716,8 @@
       <c r="P30" s="4"/>
     </row>
     <row r="31" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="43"/>
-      <c r="C31" s="42" t="s">
+      <c r="B31" s="38"/>
+      <c r="C31" s="37" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="40" t="s">
@@ -2627,10 +2726,10 @@
       <c r="E31" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="25" t="s">
+      <c r="F31" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="G31" s="25" t="s">
+      <c r="G31" s="16" t="s">
         <v>111</v>
       </c>
       <c r="I31" s="5"/>
@@ -2643,14 +2742,14 @@
       <c r="P31" s="4"/>
     </row>
     <row r="32" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="43"/>
-      <c r="C32" s="44"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="39"/>
       <c r="D32" s="41"/>
       <c r="E32" s="41"/>
-      <c r="F32" s="25" t="s">
+      <c r="F32" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="G32" s="25" t="s">
+      <c r="G32" s="16" t="s">
         <v>113</v>
       </c>
       <c r="I32" s="5"/>
@@ -2663,18 +2762,18 @@
       <c r="P32" s="4"/>
     </row>
     <row r="33" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="44"/>
-      <c r="C33" s="22" t="s">
+      <c r="B33" s="39"/>
+      <c r="C33" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="25" t="s">
+      <c r="D33" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="25" t="s">
+      <c r="E33" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -2685,16 +2784,16 @@
       <c r="P33" s="4"/>
     </row>
     <row r="34" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="C34" s="42" t="s">
+      <c r="C34" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="D34" s="24" t="s">
+      <c r="D34" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E34" s="24" t="s">
+      <c r="E34" s="15" t="s">
         <v>118</v>
       </c>
       <c r="F34" s="45"/>
@@ -2709,12 +2808,12 @@
       <c r="P34" s="4"/>
     </row>
     <row r="35" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="25" t="s">
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E35" s="25" t="s">
+      <c r="E35" s="16" t="s">
         <v>120</v>
       </c>
       <c r="F35" s="46"/>
@@ -2729,12 +2828,12 @@
       <c r="P35" s="4"/>
     </row>
     <row r="36" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="25" t="s">
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E36" s="25" t="s">
+      <c r="E36" s="16" t="s">
         <v>122</v>
       </c>
       <c r="F36" s="47"/>
@@ -3734,6 +3833,35 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="E27:E28"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C15:C16"/>
@@ -3750,35 +3878,6 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3790,8 +3889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3812,554 +3911,659 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="58" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
     </row>
     <row r="3" spans="1:19" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="29" t="s">
+      <c r="I3" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="L3" s="29" t="s">
+      <c r="L3" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="29" t="s">
+      <c r="M3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="58" t="s">
+      <c r="N3" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="59"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="58" t="s">
+      <c r="O3" s="57"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="R3" s="59"/>
-      <c r="S3" s="60"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="58"/>
     </row>
     <row r="4" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="22">
         <v>2</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="22">
         <v>12</v>
       </c>
-      <c r="J4" s="31" t="s">
+      <c r="J4" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="K4" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="L4" s="31" t="s">
+      <c r="L4" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="M4" s="31" t="s">
+      <c r="M4" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="N4" s="54" t="s">
+      <c r="N4" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="O4" s="55"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="54" t="s">
+      <c r="O4" s="50"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="R4" s="55"/>
-      <c r="S4" s="56"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="51"/>
     </row>
     <row r="5" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="24">
         <v>50</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="J5" s="33" t="s">
+      <c r="J5" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="K5" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="L5" s="33" t="s">
+      <c r="L5" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="M5" s="33" t="s">
+      <c r="M5" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="N5" s="54" t="s">
+      <c r="N5" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="O5" s="55"/>
-      <c r="P5" s="56"/>
-      <c r="Q5" s="54" t="s">
+      <c r="O5" s="50"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="R5" s="55"/>
-      <c r="S5" s="56"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="51"/>
     </row>
     <row r="6" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="H6" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="I6" s="35">
+      <c r="I6" s="26">
         <v>5</v>
       </c>
-      <c r="J6" s="35" t="s">
+      <c r="J6" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="K6" s="35" t="s">
+      <c r="K6" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="L6" s="35" t="s">
+      <c r="L6" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="M6" s="35" t="s">
+      <c r="M6" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="N6" s="54" t="s">
+      <c r="N6" s="49" t="s">
         <v>151</v>
       </c>
-      <c r="O6" s="55"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="54" t="s">
+      <c r="O6" s="50"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="R6" s="55"/>
-      <c r="S6" s="56"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="51"/>
     </row>
     <row r="7" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="28">
         <v>9.9999999999999901E+36</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="I7" s="37">
+      <c r="I7" s="28">
         <v>3</v>
       </c>
-      <c r="J7" s="37" t="s">
+      <c r="J7" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="L7" s="37" t="s">
+      <c r="L7" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="M7" s="37" t="s">
+      <c r="M7" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="N7" s="54" t="s">
+      <c r="N7" s="49" t="s">
         <v>159</v>
       </c>
-      <c r="O7" s="55"/>
-      <c r="P7" s="56"/>
-      <c r="Q7" s="54" t="s">
+      <c r="O7" s="50"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="R7" s="55"/>
-      <c r="S7" s="56"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="51"/>
     </row>
     <row r="8" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="28">
         <v>0</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="I8" s="37">
+      <c r="I8" s="28">
         <v>5</v>
       </c>
-      <c r="J8" s="37" t="s">
+      <c r="J8" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="K8" s="37" t="s">
+      <c r="K8" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="L8" s="37" t="s">
+      <c r="L8" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="M8" s="37" t="s">
+      <c r="M8" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="N8" s="54" t="s">
+      <c r="N8" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="O8" s="55"/>
-      <c r="P8" s="56"/>
-      <c r="Q8" s="54" t="s">
+      <c r="O8" s="50"/>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="R8" s="55"/>
-      <c r="S8" s="56"/>
+      <c r="R8" s="50"/>
+      <c r="S8" s="51"/>
     </row>
     <row r="9" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="D9" s="62">
+      <c r="D9" s="32">
         <v>10</v>
       </c>
-      <c r="E9" s="62">
+      <c r="E9" s="32">
         <v>-54</v>
       </c>
-      <c r="F9" s="62" t="s">
+      <c r="F9" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="G9" s="62" t="s">
+      <c r="G9" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="H9" s="62" t="s">
+      <c r="H9" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="I9" s="62">
+      <c r="I9" s="32">
         <v>7</v>
       </c>
-      <c r="J9" s="62" t="s">
+      <c r="J9" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="K9" s="62" t="s">
+      <c r="K9" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="L9" s="62" t="s">
+      <c r="L9" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="M9" s="62" t="s">
+      <c r="M9" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="N9" s="65" t="s">
+      <c r="N9" s="52" t="s">
         <v>136</v>
       </c>
-      <c r="O9" s="66"/>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="54" t="s">
+      <c r="O9" s="53"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="49" t="s">
         <v>175</v>
       </c>
-      <c r="R9" s="55"/>
-      <c r="S9" s="56"/>
+      <c r="R9" s="50"/>
+      <c r="S9" s="51"/>
     </row>
     <row r="10" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="63" t="s">
+      <c r="A10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="34">
         <v>12</v>
       </c>
-      <c r="E10" s="64" t="s">
+      <c r="E10" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="F10" s="64" t="s">
+      <c r="F10" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="G10" s="64" t="s">
+      <c r="G10" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="H10" s="64" t="s">
+      <c r="H10" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="I10" s="64">
+      <c r="I10" s="34">
         <v>8</v>
       </c>
-      <c r="J10" s="64" t="s">
+      <c r="J10" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="K10" s="64" t="s">
+      <c r="K10" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="L10" s="64" t="s">
+      <c r="L10" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="M10" s="64" t="s">
+      <c r="M10" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="N10" s="65" t="s">
+      <c r="N10" s="52" t="s">
         <v>136</v>
       </c>
-      <c r="O10" s="66"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="54" t="s">
+      <c r="O10" s="53"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="49" t="s">
         <v>183</v>
       </c>
-      <c r="R10" s="55"/>
-      <c r="S10" s="56"/>
+      <c r="R10" s="50"/>
+      <c r="S10" s="51"/>
     </row>
     <row r="11" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="D11" s="64">
+      <c r="D11" s="34">
         <v>51</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="34" t="s">
         <v>186</v>
       </c>
-      <c r="G11" s="64" t="s">
+      <c r="G11" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="H11" s="64" t="s">
+      <c r="H11" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="I11" s="64">
+      <c r="I11" s="34">
         <v>10</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="K11" s="64" t="s">
+      <c r="K11" s="34" t="s">
         <v>190</v>
       </c>
-      <c r="L11" s="64" t="s">
+      <c r="L11" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="M11" s="64" t="s">
+      <c r="M11" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="N11" s="54" t="s">
+      <c r="N11" s="49" t="s">
         <v>191</v>
       </c>
-      <c r="O11" s="55"/>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="54" t="s">
+      <c r="O11" s="50"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="R11" s="55"/>
-      <c r="S11" s="56"/>
+      <c r="R11" s="50"/>
+      <c r="S11" s="51"/>
     </row>
-    <row r="12" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
+      <c r="B12" s="60" t="s">
+        <v>192</v>
+      </c>
+      <c r="C12" s="60" t="s">
+        <v>193</v>
+      </c>
+      <c r="D12" s="60">
+        <v>41</v>
+      </c>
+      <c r="E12" s="60" t="s">
+        <v>194</v>
+      </c>
+      <c r="F12" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="G12" s="60" t="s">
+        <v>196</v>
+      </c>
+      <c r="H12" s="60" t="s">
+        <v>131</v>
+      </c>
+      <c r="I12" s="60">
+        <v>11</v>
+      </c>
+      <c r="J12" s="60" t="s">
+        <v>181</v>
+      </c>
+      <c r="K12" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="L12" s="60" t="s">
+        <v>134</v>
+      </c>
+      <c r="M12" s="60" t="s">
+        <v>150</v>
+      </c>
+      <c r="N12" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="O12" s="53"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="R12" s="50"/>
+      <c r="S12" s="51"/>
     </row>
-    <row r="13" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+      <c r="B13" s="62" t="s">
+        <v>192</v>
+      </c>
+      <c r="C13" s="62" t="s">
+        <v>198</v>
+      </c>
+      <c r="D13" s="62">
+        <v>2</v>
+      </c>
+      <c r="E13" s="62" t="s">
+        <v>199</v>
+      </c>
+      <c r="F13" s="62" t="s">
+        <v>200</v>
+      </c>
+      <c r="G13" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="H13" s="62" t="s">
+        <v>202</v>
+      </c>
+      <c r="I13" s="62">
+        <v>5</v>
+      </c>
+      <c r="J13" s="62" t="s">
+        <v>203</v>
+      </c>
+      <c r="K13" s="62" t="s">
+        <v>204</v>
+      </c>
+      <c r="L13" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="M13" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="N13" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="O13" s="53"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="R13" s="50"/>
+      <c r="S13" s="51"/>
     </row>
-    <row r="14" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
+      <c r="B14" s="62" t="s">
+        <v>192</v>
+      </c>
+      <c r="C14" s="62" t="s">
+        <v>206</v>
+      </c>
+      <c r="D14" s="62">
+        <v>14</v>
+      </c>
+      <c r="E14" s="62" t="s">
+        <v>207</v>
+      </c>
+      <c r="F14" s="62" t="s">
+        <v>208</v>
+      </c>
+      <c r="G14" s="62" t="s">
+        <v>209</v>
+      </c>
+      <c r="H14" s="62" t="s">
+        <v>156</v>
+      </c>
+      <c r="I14" s="62">
+        <v>6</v>
+      </c>
+      <c r="J14" s="62" t="s">
+        <v>210</v>
+      </c>
+      <c r="K14" s="62" t="s">
+        <v>203</v>
+      </c>
+      <c r="L14" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="M14" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="N14" s="49" t="s">
+        <v>211</v>
+      </c>
+      <c r="O14" s="50"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="R14" s="50"/>
+      <c r="S14" s="51"/>
     </row>
     <row r="15" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="18"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5338,7 +5542,19 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="26">
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="Q11:S11"/>
     <mergeCell ref="N5:P5"/>
@@ -5347,12 +5563,6 @@
     <mergeCell ref="Q9:S9"/>
     <mergeCell ref="N10:P10"/>
     <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
     <mergeCell ref="N6:P6"/>
     <mergeCell ref="Q6:S6"/>
     <mergeCell ref="N7:P7"/>

</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas Urbanizacion incorrectas se reporta errores en el CP12 y CP13
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD020C9D-584D-4FEA-8F83-FB657E5AE26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E5CF48-222D-47DD-BBC8-881F2F0C701F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="235">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -1213,12 +1213,142 @@
   <si>
     <t>No se permite el ingreso de "fsdsgfdsgds,,,,," como Nombres</t>
   </si>
+  <si>
+    <t>Registro con Urbanización Incorrecto</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;10&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;09&gt; , CEV&lt;12&gt; , CEV&lt;14&gt; , CEV&lt;17&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Ruiz</t>
+  </si>
+  <si>
+    <t>Anaís</t>
+  </si>
+  <si>
+    <t>150/-</t>
+  </si>
+  <si>
+    <t>Paita</t>
+  </si>
+  <si>
+    <t>Huancavelica</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir números y carácteres no alfanuméricos como Urbanización</t>
+  </si>
+  <si>
+    <t>CP13</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;11&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;09&gt; , CEV&lt;12&gt; , CEV&lt;14&gt; , CEV&lt;17&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Sánchez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucas 
+</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Ayabaca</t>
+  </si>
+  <si>
+    <t>Acobamba</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir Urbanización de una letra</t>
+  </si>
+  <si>
+    <t>CP14</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;12&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;11&gt; ,CEV&lt;16&gt; , CEV&lt;14&gt; , CEV&lt;19&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Ramírez</t>
+  </si>
+  <si>
+    <t>Eva</t>
+  </si>
+  <si>
+    <t>ehrdrehhreherherhretgertergerg5regerhrehfdhdfhthtrhrthtrjdfhdfgsdegrewgweegwsgegwegewgew</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "ehrdrehhreherherhre,,,,," como Urbanización</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1249,27 +1379,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1338,12 +1447,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9FC5E8"/>
-        <bgColor rgb="FF9FC5E8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1375,6 +1478,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE6B8AF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FC5E8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1615,106 +1724,118 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1722,56 +1843,44 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2204,14 +2313,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="35" t="s">
+      <c r="E3" s="45"/>
+      <c r="F3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="45"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -2246,10 +2355,10 @@
       <c r="E5" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2258,10 +2367,10 @@
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2270,10 +2379,10 @@
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
       <c r="E7" s="39"/>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2281,19 +2390,19 @@
       <c r="B8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2302,28 +2411,28 @@
       <c r="C9" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="39"/>
       <c r="C10" s="39"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="16" t="s">
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="12" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2331,19 +2440,19 @@
       <c r="B11" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="11" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2352,28 +2461,28 @@
       <c r="C12" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="16" t="s">
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="12" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2381,19 +2490,19 @@
       <c r="B14" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="11" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2402,62 +2511,62 @@
       <c r="C15" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="38"/>
       <c r="C16" s="39"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="16" t="s">
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="12" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="39"/>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="11" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2466,40 +2575,40 @@
       <c r="C19" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="40" t="s">
+      <c r="G19" s="35" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="38"/>
       <c r="C20" s="39"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
     </row>
     <row r="21" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="39"/>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="37" t="s">
@@ -2508,36 +2617,36 @@
       <c r="C22" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="11" t="s">
         <v>85</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="43"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="47"/>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="16" t="s">
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="G23" s="12" t="s">
         <v>87</v>
       </c>
       <c r="I23" s="5"/>
@@ -2552,12 +2661,12 @@
     <row r="24" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="38"/>
       <c r="C24" s="39"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="16" t="s">
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="G24" s="16" t="s">
+      <c r="G24" s="12" t="s">
         <v>89</v>
       </c>
       <c r="I24" s="5"/>
@@ -2566,48 +2675,48 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="42"/>
+      <c r="O24" s="46"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="39"/>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="43"/>
+      <c r="O25" s="47"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="11" t="s">
         <v>95</v>
       </c>
       <c r="I26" s="5"/>
@@ -2616,7 +2725,7 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="42"/>
+      <c r="O26" s="46"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2624,16 +2733,16 @@
       <c r="C27" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="E27" s="40" t="s">
+      <c r="E27" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="12" t="s">
         <v>99</v>
       </c>
       <c r="I27" s="5"/>
@@ -2642,18 +2751,18 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="43"/>
+      <c r="O27" s="47"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="38"/>
       <c r="C28" s="39"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="16" t="s">
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="G28" s="16" t="s">
+      <c r="G28" s="12" t="s">
         <v>101</v>
       </c>
       <c r="I28" s="5"/>
@@ -2662,48 +2771,48 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="42"/>
+      <c r="O28" s="46"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="39"/>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="43"/>
+      <c r="O29" s="47"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="G30" s="15" t="s">
+      <c r="G30" s="11" t="s">
         <v>107</v>
       </c>
       <c r="I30" s="5"/>
@@ -2720,16 +2829,16 @@
       <c r="C31" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="40" t="s">
+      <c r="E31" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F31" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="G31" s="16" t="s">
+      <c r="G31" s="12" t="s">
         <v>111</v>
       </c>
       <c r="I31" s="5"/>
@@ -2744,12 +2853,12 @@
     <row r="32" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="38"/>
       <c r="C32" s="39"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="16" t="s">
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="G32" s="12" t="s">
         <v>113</v>
       </c>
       <c r="I32" s="5"/>
@@ -2763,17 +2872,17 @@
     </row>
     <row r="33" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="39"/>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -2790,14 +2899,14 @@
       <c r="C34" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -2810,14 +2919,14 @@
     <row r="35" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="38"/>
       <c r="C35" s="38"/>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="E35" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="F35" s="46"/>
-      <c r="G35" s="46"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -2830,14 +2939,14 @@
     <row r="36" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="39"/>
       <c r="C36" s="39"/>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E36" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -3833,6 +3942,35 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="O26:O27"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="C34:C36"/>
@@ -3849,35 +3987,6 @@
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="E22:E24"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3890,7 +3999,7 @@
   <dimension ref="A1:S991"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3914,13 +4023,13 @@
       <c r="A1" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="17"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="13"/>
       <c r="D2" s="56" t="s">
         <v>6</v>
       </c>
@@ -3932,52 +4041,52 @@
       <c r="J2" s="57"/>
       <c r="K2" s="57"/>
       <c r="L2" s="58"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
     </row>
     <row r="3" spans="1:19" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="16" t="s">
         <v>9</v>
       </c>
       <c r="N3" s="56" t="s">
@@ -3992,596 +4101,734 @@
       <c r="S3" s="58"/>
     </row>
     <row r="4" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="18">
         <v>2</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="18">
         <v>12</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="L4" s="22" t="s">
+      <c r="L4" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="N4" s="49" t="s">
+      <c r="N4" s="52" t="s">
         <v>136</v>
       </c>
-      <c r="O4" s="50"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="49" t="s">
+      <c r="O4" s="53"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="R4" s="50"/>
-      <c r="S4" s="51"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="54"/>
     </row>
     <row r="5" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="20">
         <v>50</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="L5" s="24" t="s">
+      <c r="L5" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="M5" s="24" t="s">
+      <c r="M5" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="N5" s="49" t="s">
+      <c r="N5" s="52" t="s">
         <v>136</v>
       </c>
-      <c r="O5" s="50"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="49" t="s">
+      <c r="O5" s="53"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="R5" s="50"/>
-      <c r="S5" s="51"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="54"/>
     </row>
     <row r="6" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="22">
         <v>5</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="L6" s="26" t="s">
+      <c r="L6" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="M6" s="26" t="s">
+      <c r="M6" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="N6" s="49" t="s">
+      <c r="N6" s="52" t="s">
         <v>151</v>
       </c>
-      <c r="O6" s="50"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="49" t="s">
+      <c r="O6" s="53"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="R6" s="50"/>
-      <c r="S6" s="51"/>
+      <c r="R6" s="53"/>
+      <c r="S6" s="54"/>
     </row>
     <row r="7" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="24">
         <v>9.9999999999999901E+36</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="I7" s="28">
+      <c r="I7" s="24">
         <v>3</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="K7" s="28" t="s">
+      <c r="K7" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="L7" s="28" t="s">
+      <c r="L7" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="M7" s="28" t="s">
+      <c r="M7" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="N7" s="49" t="s">
+      <c r="N7" s="52" t="s">
         <v>159</v>
       </c>
-      <c r="O7" s="50"/>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="49" t="s">
+      <c r="O7" s="53"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="R7" s="50"/>
-      <c r="S7" s="51"/>
+      <c r="R7" s="53"/>
+      <c r="S7" s="54"/>
     </row>
     <row r="8" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="24">
         <v>0</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="24">
         <v>5</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="K8" s="28" t="s">
+      <c r="K8" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="L8" s="28" t="s">
+      <c r="L8" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="M8" s="28" t="s">
+      <c r="M8" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="N8" s="49" t="s">
+      <c r="N8" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="O8" s="50"/>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="49" t="s">
+      <c r="O8" s="53"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="R8" s="50"/>
-      <c r="S8" s="51"/>
+      <c r="R8" s="53"/>
+      <c r="S8" s="54"/>
     </row>
     <row r="9" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="28">
         <v>10</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="28">
         <v>-54</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="28">
         <v>7</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="K9" s="32" t="s">
+      <c r="K9" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="L9" s="32" t="s">
+      <c r="L9" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="M9" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="N9" s="52" t="s">
+      <c r="N9" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="O9" s="53"/>
-      <c r="P9" s="54"/>
-      <c r="Q9" s="49" t="s">
+      <c r="O9" s="50"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="52" t="s">
         <v>175</v>
       </c>
-      <c r="R9" s="50"/>
-      <c r="S9" s="51"/>
+      <c r="R9" s="53"/>
+      <c r="S9" s="54"/>
     </row>
     <row r="10" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="30">
         <v>12</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="G10" s="34" t="s">
+      <c r="G10" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="H10" s="34" t="s">
+      <c r="H10" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="I10" s="34">
+      <c r="I10" s="30">
         <v>8</v>
       </c>
-      <c r="J10" s="34" t="s">
+      <c r="J10" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="K10" s="34" t="s">
+      <c r="K10" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="L10" s="34" t="s">
+      <c r="L10" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="M10" s="34" t="s">
+      <c r="M10" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="N10" s="52" t="s">
+      <c r="N10" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="O10" s="53"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="49" t="s">
+      <c r="O10" s="50"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="52" t="s">
         <v>183</v>
       </c>
-      <c r="R10" s="50"/>
-      <c r="S10" s="51"/>
+      <c r="R10" s="53"/>
+      <c r="S10" s="54"/>
     </row>
     <row r="11" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="30">
         <v>51</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="I11" s="34">
+      <c r="I11" s="30">
         <v>10</v>
       </c>
-      <c r="J11" s="34" t="s">
+      <c r="J11" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="K11" s="34" t="s">
+      <c r="K11" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="L11" s="34" t="s">
+      <c r="L11" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="M11" s="34" t="s">
+      <c r="M11" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="N11" s="49" t="s">
+      <c r="N11" s="52" t="s">
         <v>191</v>
       </c>
-      <c r="O11" s="50"/>
-      <c r="P11" s="51"/>
-      <c r="Q11" s="49" t="s">
+      <c r="O11" s="53"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="R11" s="50"/>
-      <c r="S11" s="51"/>
+      <c r="R11" s="53"/>
+      <c r="S11" s="54"/>
     </row>
     <row r="12" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C12" s="60" t="s">
+      <c r="C12" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="D12" s="60">
+      <c r="D12" s="32">
         <v>41</v>
       </c>
-      <c r="E12" s="60" t="s">
+      <c r="E12" s="32" t="s">
         <v>194</v>
       </c>
-      <c r="F12" s="60" t="s">
+      <c r="F12" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="G12" s="60" t="s">
+      <c r="G12" s="32" t="s">
         <v>196</v>
       </c>
-      <c r="H12" s="60" t="s">
+      <c r="H12" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="I12" s="60">
+      <c r="I12" s="32">
         <v>11</v>
       </c>
-      <c r="J12" s="60" t="s">
+      <c r="J12" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="K12" s="60" t="s">
+      <c r="K12" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="L12" s="60" t="s">
+      <c r="L12" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="M12" s="60" t="s">
+      <c r="M12" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="N12" s="52" t="s">
+      <c r="N12" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="O12" s="53"/>
-      <c r="P12" s="54"/>
-      <c r="Q12" s="49" t="s">
+      <c r="O12" s="50"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="52" t="s">
         <v>197</v>
       </c>
-      <c r="R12" s="50"/>
-      <c r="S12" s="51"/>
+      <c r="R12" s="53"/>
+      <c r="S12" s="54"/>
     </row>
     <row r="13" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="C13" s="62" t="s">
+      <c r="C13" s="34" t="s">
         <v>198</v>
       </c>
-      <c r="D13" s="62">
+      <c r="D13" s="34">
         <v>2</v>
       </c>
-      <c r="E13" s="62" t="s">
+      <c r="E13" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="F13" s="62" t="s">
+      <c r="F13" s="34" t="s">
         <v>200</v>
       </c>
-      <c r="G13" s="62" t="s">
+      <c r="G13" s="34" t="s">
         <v>201</v>
       </c>
-      <c r="H13" s="62" t="s">
+      <c r="H13" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="I13" s="62">
+      <c r="I13" s="34">
         <v>5</v>
       </c>
-      <c r="J13" s="62" t="s">
+      <c r="J13" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="K13" s="62" t="s">
+      <c r="K13" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="L13" s="62" t="s">
+      <c r="L13" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="M13" s="62" t="s">
+      <c r="M13" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="N13" s="52" t="s">
+      <c r="N13" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="O13" s="53"/>
-      <c r="P13" s="54"/>
-      <c r="Q13" s="49" t="s">
+      <c r="O13" s="50"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="52" t="s">
         <v>205</v>
       </c>
-      <c r="R13" s="50"/>
-      <c r="S13" s="51"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="54"/>
     </row>
     <row r="14" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="C14" s="62" t="s">
+      <c r="C14" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D14" s="62">
+      <c r="D14" s="34">
         <v>14</v>
       </c>
-      <c r="E14" s="62" t="s">
+      <c r="E14" s="34" t="s">
         <v>207</v>
       </c>
-      <c r="F14" s="62" t="s">
+      <c r="F14" s="34" t="s">
         <v>208</v>
       </c>
-      <c r="G14" s="62" t="s">
+      <c r="G14" s="34" t="s">
         <v>209</v>
       </c>
-      <c r="H14" s="62" t="s">
+      <c r="H14" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="I14" s="62">
+      <c r="I14" s="34">
         <v>6</v>
       </c>
-      <c r="J14" s="62" t="s">
+      <c r="J14" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="K14" s="62" t="s">
+      <c r="K14" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="L14" s="62" t="s">
+      <c r="L14" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="M14" s="62" t="s">
+      <c r="M14" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="N14" s="49" t="s">
+      <c r="N14" s="52" t="s">
         <v>211</v>
       </c>
-      <c r="O14" s="50"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="49" t="s">
+      <c r="O14" s="53"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="R14" s="50"/>
-      <c r="S14" s="51"/>
+      <c r="R14" s="53"/>
+      <c r="S14" s="54"/>
     </row>
-    <row r="15" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="9"/>
+      <c r="B15" s="60" t="s">
+        <v>212</v>
+      </c>
+      <c r="C15" s="60" t="s">
+        <v>213</v>
+      </c>
+      <c r="D15" s="60">
+        <v>54</v>
+      </c>
+      <c r="E15" s="60" t="s">
+        <v>214</v>
+      </c>
+      <c r="F15" s="60" t="s">
+        <v>215</v>
+      </c>
+      <c r="G15" s="60" t="s">
+        <v>216</v>
+      </c>
+      <c r="H15" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="I15" s="60">
+        <v>77</v>
+      </c>
+      <c r="J15" s="60" t="s">
+        <v>217</v>
+      </c>
+      <c r="K15" s="60" t="s">
+        <v>218</v>
+      </c>
+      <c r="L15" s="60" t="s">
+        <v>134</v>
+      </c>
+      <c r="M15" s="60" t="s">
+        <v>150</v>
+      </c>
+      <c r="N15" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="O15" s="50"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="52" t="s">
+        <v>219</v>
+      </c>
+      <c r="R15" s="53"/>
+      <c r="S15" s="54"/>
     </row>
-    <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:19" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="61" t="s">
+        <v>220</v>
+      </c>
+      <c r="B16" s="62" t="s">
+        <v>212</v>
+      </c>
+      <c r="C16" s="62" t="s">
+        <v>221</v>
+      </c>
+      <c r="D16" s="62">
+        <v>46</v>
+      </c>
+      <c r="E16" s="62" t="s">
+        <v>222</v>
+      </c>
+      <c r="F16" s="62" t="s">
+        <v>223</v>
+      </c>
+      <c r="G16" s="62" t="s">
+        <v>224</v>
+      </c>
+      <c r="H16" s="62" t="s">
+        <v>225</v>
+      </c>
+      <c r="I16" s="62">
+        <v>88</v>
+      </c>
+      <c r="J16" s="62" t="s">
+        <v>226</v>
+      </c>
+      <c r="K16" s="62" t="s">
+        <v>227</v>
+      </c>
+      <c r="L16" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="M16" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="N16" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="O16" s="50"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="52" t="s">
+        <v>228</v>
+      </c>
+      <c r="R16" s="53"/>
+      <c r="S16" s="54"/>
+    </row>
+    <row r="17" spans="1:19" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="61" t="s">
+        <v>229</v>
+      </c>
+      <c r="B17" s="62" t="s">
+        <v>212</v>
+      </c>
+      <c r="C17" s="62" t="s">
+        <v>230</v>
+      </c>
+      <c r="D17" s="62">
+        <v>2</v>
+      </c>
+      <c r="E17" s="62" t="s">
+        <v>231</v>
+      </c>
+      <c r="F17" s="62" t="s">
+        <v>232</v>
+      </c>
+      <c r="G17" s="62" t="s">
+        <v>233</v>
+      </c>
+      <c r="H17" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="I17" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="J17" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="K17" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="L17" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="M17" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="N17" s="52" t="s">
+        <v>234</v>
+      </c>
+      <c r="O17" s="53"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="R17" s="53"/>
+      <c r="S17" s="54"/>
+    </row>
+    <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5542,19 +5789,13 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
+  <mergeCells count="32">
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="Q11:S11"/>
     <mergeCell ref="N5:P5"/>
@@ -5569,6 +5810,18 @@
     <mergeCell ref="Q7:S7"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="Q14:S14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas Manzana incorrectas se reporta errores en el CP15
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E5CF48-222D-47DD-BBC8-881F2F0C701F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B436453-062B-4A62-A263-F73E4B0142E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="246">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -1342,6 +1342,79 @@
   </si>
   <si>
     <t>No se permite el ingreso de "ehrdrehhreherherhre,,,,," como Urbanización</t>
+  </si>
+  <si>
+    <t>CP15</t>
+  </si>
+  <si>
+    <t>Registro con Manzana Incorrecto</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;08&gt; ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;13&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ,CEV&lt;16&gt; , CEV&lt;14&gt; , CEV&lt;19&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Jiménez</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir números y carácteres no alfanuméricos como Manzana</t>
+  </si>
+  <si>
+    <t>CP16</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;08&gt; ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;14&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ,CEV&lt;16&gt; , CEV&lt;14&gt; , CEV&lt;19&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Romero</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>fbf</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "fbf" como Manzana</t>
   </si>
 </sst>
 </file>
@@ -1426,7 +1499,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1484,6 +1557,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF9FC5E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE5CD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1703,7 +1782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1805,37 +1884,37 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1843,6 +1922,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1871,16 +1962,16 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2313,14 +2404,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="44" t="s">
+      <c r="E3" s="40"/>
+      <c r="F3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="45"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -2343,16 +2434,16 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="41" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -2363,10 +2454,10 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
       <c r="F6" s="9" t="s">
         <v>29</v>
       </c>
@@ -2375,10 +2466,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
       <c r="F7" s="9" t="s">
         <v>31</v>
       </c>
@@ -2387,7 +2478,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="41" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -2407,14 +2498,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="38"/>
-      <c r="C9" s="37" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="44" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="12" t="s">
@@ -2425,10 +2516,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="12" t="s">
         <v>44</v>
       </c>
@@ -2437,7 +2528,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="41" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -2457,14 +2548,14 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="38"/>
-      <c r="C12" s="37" t="s">
+      <c r="B12" s="42"/>
+      <c r="C12" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="44" t="s">
         <v>52</v>
       </c>
       <c r="F12" s="12" t="s">
@@ -2475,10 +2566,10 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="12" t="s">
         <v>55</v>
       </c>
@@ -2487,7 +2578,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="41" t="s">
         <v>57</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -2507,14 +2598,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="38"/>
-      <c r="C15" s="37" t="s">
+      <c r="B15" s="42"/>
+      <c r="C15" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="44" t="s">
         <v>63</v>
       </c>
       <c r="F15" s="12" t="s">
@@ -2525,10 +2616,10 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
       <c r="F16" s="12" t="s">
         <v>66</v>
       </c>
@@ -2537,7 +2628,7 @@
       </c>
     </row>
     <row r="17" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="39"/>
+      <c r="B17" s="43"/>
       <c r="C17" s="9" t="s">
         <v>34</v>
       </c>
@@ -2551,7 +2642,7 @@
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="41" t="s">
         <v>70</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -2571,33 +2662,33 @@
       </c>
     </row>
     <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="38"/>
-      <c r="C19" s="37" t="s">
+      <c r="B19" s="42"/>
+      <c r="C19" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="35" t="s">
+      <c r="F19" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="35" t="s">
+      <c r="G19" s="44" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
     </row>
     <row r="21" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="39"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="9" t="s">
         <v>34</v>
       </c>
@@ -2611,16 +2702,16 @@
       <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="44" t="s">
         <v>83</v>
       </c>
       <c r="F22" s="11" t="s">
@@ -2639,10 +2730,10 @@
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
       <c r="F23" s="12" t="s">
         <v>86</v>
       </c>
@@ -2659,10 +2750,10 @@
       <c r="P23" s="4"/>
     </row>
     <row r="24" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="38"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
       <c r="F24" s="12" t="s">
         <v>88</v>
       </c>
@@ -2679,7 +2770,7 @@
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="39"/>
+      <c r="B25" s="43"/>
       <c r="C25" s="9" t="s">
         <v>34</v>
       </c>
@@ -2701,7 +2792,7 @@
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="41" t="s">
         <v>91</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -2729,14 +2820,14 @@
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="38"/>
-      <c r="C27" s="37" t="s">
+      <c r="B27" s="42"/>
+      <c r="C27" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="E27" s="35" t="s">
+      <c r="E27" s="44" t="s">
         <v>97</v>
       </c>
       <c r="F27" s="12" t="s">
@@ -2755,10 +2846,10 @@
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="38"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
       <c r="F28" s="12" t="s">
         <v>100</v>
       </c>
@@ -2775,7 +2866,7 @@
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="39"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="9" t="s">
         <v>34</v>
       </c>
@@ -2797,7 +2888,7 @@
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="41" t="s">
         <v>103</v>
       </c>
       <c r="C30" s="10" t="s">
@@ -2825,14 +2916,14 @@
       <c r="P30" s="4"/>
     </row>
     <row r="31" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="38"/>
-      <c r="C31" s="37" t="s">
+      <c r="B31" s="42"/>
+      <c r="C31" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D31" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="44" t="s">
         <v>109</v>
       </c>
       <c r="F31" s="12" t="s">
@@ -2851,10 +2942,10 @@
       <c r="P31" s="4"/>
     </row>
     <row r="32" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="38"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
       <c r="F32" s="12" t="s">
         <v>112</v>
       </c>
@@ -2871,7 +2962,7 @@
       <c r="P32" s="4"/>
     </row>
     <row r="33" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="39"/>
+      <c r="B33" s="43"/>
       <c r="C33" s="9" t="s">
         <v>34</v>
       </c>
@@ -2893,10 +2984,10 @@
       <c r="P33" s="4"/>
     </row>
     <row r="34" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="C34" s="37" t="s">
+      <c r="C34" s="41" t="s">
         <v>116</v>
       </c>
       <c r="D34" s="11" t="s">
@@ -2905,8 +2996,8 @@
       <c r="E34" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -2917,16 +3008,16 @@
       <c r="P34" s="4"/>
     </row>
     <row r="35" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
       <c r="D35" s="12" t="s">
         <v>119</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -2937,16 +3028,16 @@
       <c r="P35" s="4"/>
     </row>
     <row r="36" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="39"/>
-      <c r="C36" s="39"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
       <c r="D36" s="12" t="s">
         <v>121</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -3942,6 +4033,35 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="E27:E28"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C15:C16"/>
@@ -3958,35 +4078,6 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3998,8 +4089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4020,7 +4111,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="59" t="s">
         <v>123</v>
       </c>
       <c r="B1" s="47"/>
@@ -4030,17 +4121,17 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="13"/>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="58"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="62"/>
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
@@ -4089,16 +4180,16 @@
       <c r="M3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="56" t="s">
+      <c r="N3" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="57"/>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="56" t="s">
+      <c r="O3" s="61"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="60" t="s">
         <v>125</v>
       </c>
-      <c r="R3" s="57"/>
-      <c r="S3" s="58"/>
+      <c r="R3" s="61"/>
+      <c r="S3" s="62"/>
     </row>
     <row r="4" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
@@ -4140,16 +4231,16 @@
       <c r="M4" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="N4" s="52" t="s">
+      <c r="N4" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="O4" s="53"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="52" t="s">
+      <c r="O4" s="57"/>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="R4" s="53"/>
-      <c r="S4" s="54"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="58"/>
     </row>
     <row r="5" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
@@ -4191,16 +4282,16 @@
       <c r="M5" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="N5" s="52" t="s">
+      <c r="N5" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="O5" s="53"/>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="52" t="s">
+      <c r="O5" s="57"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="R5" s="53"/>
-      <c r="S5" s="54"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="58"/>
     </row>
     <row r="6" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
@@ -4242,16 +4333,16 @@
       <c r="M6" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="N6" s="52" t="s">
+      <c r="N6" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="O6" s="53"/>
-      <c r="P6" s="54"/>
-      <c r="Q6" s="52" t="s">
+      <c r="O6" s="57"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="R6" s="53"/>
-      <c r="S6" s="54"/>
+      <c r="R6" s="57"/>
+      <c r="S6" s="58"/>
     </row>
     <row r="7" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -4293,16 +4384,16 @@
       <c r="M7" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="N7" s="52" t="s">
+      <c r="N7" s="56" t="s">
         <v>159</v>
       </c>
-      <c r="O7" s="53"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="52" t="s">
+      <c r="O7" s="57"/>
+      <c r="P7" s="58"/>
+      <c r="Q7" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="R7" s="53"/>
-      <c r="S7" s="54"/>
+      <c r="R7" s="57"/>
+      <c r="S7" s="58"/>
     </row>
     <row r="8" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -4344,16 +4435,16 @@
       <c r="M8" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="N8" s="52" t="s">
+      <c r="N8" s="56" t="s">
         <v>167</v>
       </c>
-      <c r="O8" s="53"/>
-      <c r="P8" s="54"/>
-      <c r="Q8" s="52" t="s">
+      <c r="O8" s="57"/>
+      <c r="P8" s="58"/>
+      <c r="Q8" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="R8" s="53"/>
-      <c r="S8" s="54"/>
+      <c r="R8" s="57"/>
+      <c r="S8" s="58"/>
     </row>
     <row r="9" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
@@ -4395,16 +4486,16 @@
       <c r="M9" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="N9" s="49" t="s">
+      <c r="N9" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="O9" s="50"/>
-      <c r="P9" s="51"/>
-      <c r="Q9" s="52" t="s">
+      <c r="O9" s="54"/>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="56" t="s">
         <v>175</v>
       </c>
-      <c r="R9" s="53"/>
-      <c r="S9" s="54"/>
+      <c r="R9" s="57"/>
+      <c r="S9" s="58"/>
     </row>
     <row r="10" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
@@ -4446,16 +4537,16 @@
       <c r="M10" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="N10" s="49" t="s">
+      <c r="N10" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="O10" s="50"/>
-      <c r="P10" s="51"/>
-      <c r="Q10" s="52" t="s">
+      <c r="O10" s="54"/>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="56" t="s">
         <v>183</v>
       </c>
-      <c r="R10" s="53"/>
-      <c r="S10" s="54"/>
+      <c r="R10" s="57"/>
+      <c r="S10" s="58"/>
     </row>
     <row r="11" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
@@ -4497,16 +4588,16 @@
       <c r="M11" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="N11" s="52" t="s">
+      <c r="N11" s="56" t="s">
         <v>191</v>
       </c>
-      <c r="O11" s="53"/>
-      <c r="P11" s="54"/>
-      <c r="Q11" s="52" t="s">
+      <c r="O11" s="57"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="R11" s="53"/>
-      <c r="S11" s="54"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="58"/>
     </row>
     <row r="12" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
@@ -4548,16 +4639,16 @@
       <c r="M12" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="N12" s="49" t="s">
+      <c r="N12" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="O12" s="50"/>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="52" t="s">
+      <c r="O12" s="54"/>
+      <c r="P12" s="55"/>
+      <c r="Q12" s="56" t="s">
         <v>197</v>
       </c>
-      <c r="R12" s="53"/>
-      <c r="S12" s="54"/>
+      <c r="R12" s="57"/>
+      <c r="S12" s="58"/>
     </row>
     <row r="13" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
@@ -4599,16 +4690,16 @@
       <c r="M13" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="N13" s="49" t="s">
+      <c r="N13" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="O13" s="50"/>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="52" t="s">
+      <c r="O13" s="54"/>
+      <c r="P13" s="55"/>
+      <c r="Q13" s="56" t="s">
         <v>205</v>
       </c>
-      <c r="R13" s="53"/>
-      <c r="S13" s="54"/>
+      <c r="R13" s="57"/>
+      <c r="S13" s="58"/>
     </row>
     <row r="14" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
@@ -4650,172 +4741,272 @@
       <c r="M14" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="N14" s="52" t="s">
+      <c r="N14" s="56" t="s">
         <v>211</v>
       </c>
-      <c r="O14" s="53"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="52" t="s">
+      <c r="O14" s="57"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="R14" s="53"/>
-      <c r="S14" s="54"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="58"/>
     </row>
     <row r="15" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="C15" s="60" t="s">
+      <c r="C15" s="36" t="s">
         <v>213</v>
       </c>
-      <c r="D15" s="60">
+      <c r="D15" s="36">
         <v>54</v>
       </c>
-      <c r="E15" s="60" t="s">
+      <c r="E15" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="F15" s="60" t="s">
+      <c r="F15" s="36" t="s">
         <v>215</v>
       </c>
-      <c r="G15" s="60" t="s">
+      <c r="G15" s="36" t="s">
         <v>216</v>
       </c>
-      <c r="H15" s="60" t="s">
+      <c r="H15" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="I15" s="60">
+      <c r="I15" s="36">
         <v>77</v>
       </c>
-      <c r="J15" s="60" t="s">
+      <c r="J15" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="K15" s="60" t="s">
+      <c r="K15" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="L15" s="60" t="s">
+      <c r="L15" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="M15" s="60" t="s">
+      <c r="M15" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="N15" s="49" t="s">
+      <c r="N15" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="O15" s="50"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="52" t="s">
+      <c r="O15" s="54"/>
+      <c r="P15" s="55"/>
+      <c r="Q15" s="56" t="s">
         <v>219</v>
       </c>
-      <c r="R15" s="53"/>
-      <c r="S15" s="54"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="58"/>
     </row>
     <row r="16" spans="1:19" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="C16" s="62" t="s">
+      <c r="C16" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="D16" s="62">
+      <c r="D16" s="38">
         <v>46</v>
       </c>
-      <c r="E16" s="62" t="s">
+      <c r="E16" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="F16" s="62" t="s">
+      <c r="F16" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="G16" s="62" t="s">
+      <c r="G16" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="H16" s="62" t="s">
+      <c r="H16" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="I16" s="62">
+      <c r="I16" s="38">
         <v>88</v>
       </c>
-      <c r="J16" s="62" t="s">
+      <c r="J16" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="K16" s="62" t="s">
+      <c r="K16" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="L16" s="62" t="s">
+      <c r="L16" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="M16" s="62" t="s">
+      <c r="M16" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="N16" s="49" t="s">
+      <c r="N16" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="O16" s="50"/>
-      <c r="P16" s="51"/>
-      <c r="Q16" s="52" t="s">
+      <c r="O16" s="54"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="56" t="s">
         <v>228</v>
       </c>
-      <c r="R16" s="53"/>
-      <c r="S16" s="54"/>
+      <c r="R16" s="57"/>
+      <c r="S16" s="58"/>
     </row>
     <row r="17" spans="1:19" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="37" t="s">
         <v>229</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="C17" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="D17" s="62">
+      <c r="D17" s="38">
         <v>2</v>
       </c>
-      <c r="E17" s="62" t="s">
+      <c r="E17" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="F17" s="62" t="s">
+      <c r="F17" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="G17" s="62" t="s">
+      <c r="G17" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="H17" s="62" t="s">
+      <c r="H17" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="I17" s="62" t="s">
+      <c r="I17" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="J17" s="62" t="s">
+      <c r="J17" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="K17" s="62" t="s">
+      <c r="K17" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="L17" s="62" t="s">
+      <c r="L17" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="M17" s="62" t="s">
+      <c r="M17" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="N17" s="52" t="s">
+      <c r="N17" s="56" t="s">
         <v>234</v>
       </c>
-      <c r="O17" s="53"/>
-      <c r="P17" s="54"/>
-      <c r="Q17" s="52" t="s">
+      <c r="O17" s="57"/>
+      <c r="P17" s="58"/>
+      <c r="Q17" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="R17" s="53"/>
-      <c r="S17" s="54"/>
+      <c r="R17" s="57"/>
+      <c r="S17" s="58"/>
     </row>
-    <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="63" t="s">
+        <v>235</v>
+      </c>
+      <c r="B18" s="64" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" s="64" t="s">
+        <v>237</v>
+      </c>
+      <c r="D18" s="64">
+        <v>7</v>
+      </c>
+      <c r="E18" s="64" t="s">
+        <v>238</v>
+      </c>
+      <c r="F18" s="64" t="s">
+        <v>215</v>
+      </c>
+      <c r="G18" s="64" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" s="64">
+        <v>5</v>
+      </c>
+      <c r="I18" s="64" t="s">
+        <v>134</v>
+      </c>
+      <c r="J18" s="64" t="s">
+        <v>134</v>
+      </c>
+      <c r="K18" s="64" t="s">
+        <v>134</v>
+      </c>
+      <c r="L18" s="64" t="s">
+        <v>134</v>
+      </c>
+      <c r="M18" s="64" t="s">
+        <v>150</v>
+      </c>
+      <c r="N18" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="O18" s="54"/>
+      <c r="P18" s="55"/>
+      <c r="Q18" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="R18" s="57"/>
+      <c r="S18" s="58"/>
+    </row>
+    <row r="19" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="B19" s="66" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" s="66" t="s">
+        <v>241</v>
+      </c>
+      <c r="D19" s="66">
+        <v>8</v>
+      </c>
+      <c r="E19" s="66" t="s">
+        <v>242</v>
+      </c>
+      <c r="F19" s="66" t="s">
+        <v>243</v>
+      </c>
+      <c r="G19" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="H19" s="66" t="s">
+        <v>244</v>
+      </c>
+      <c r="I19" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="J19" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="K19" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="L19" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="M19" s="66" t="s">
+        <v>150</v>
+      </c>
+      <c r="N19" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="O19" s="57"/>
+      <c r="P19" s="58"/>
+      <c r="Q19" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="R19" s="57"/>
+      <c r="S19" s="58"/>
+    </row>
     <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5789,13 +5980,23 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
+  <mergeCells count="36">
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="Q11:S11"/>
     <mergeCell ref="N5:P5"/>
@@ -5810,18 +6011,12 @@
     <mergeCell ref="Q7:S7"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas Lote incorrectas se reporta errores en el CP18
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B436453-062B-4A62-A263-F73E4B0142E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60548168-D88A-4DC1-8C9A-FAFD38A81FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="261">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -1415,6 +1415,111 @@
   </si>
   <si>
     <t>No se permite el ingreso de "fbf" como Manzana</t>
+  </si>
+  <si>
+    <t>CP17</t>
+  </si>
+  <si>
+    <t>Registro con Lote Incorrecto</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;08&gt; ,CEV&lt;11&gt; ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;15&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> , CEV&lt;14&gt; , CEV&lt;19&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Medina</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "A" como Lote</t>
+  </si>
+  <si>
+    <t>CP18</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;08&gt; ,CEV&lt;11&gt; ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;16&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, CEV&lt;14&gt; , CEV&lt;19&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Herrera</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Error no se debe adminitr un número de lote menor igual a 0</t>
+  </si>
+  <si>
+    <t>CP19</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;08&gt; ,CEV&lt;11&gt; ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;17&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> , CEV&lt;14&gt; , CEV&lt;19&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Castro</t>
+  </si>
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "5225" como Lote</t>
   </si>
 </sst>
 </file>
@@ -1499,7 +1604,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1563,6 +1668,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCE5CD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1782,7 +1893,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1896,25 +2007,49 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1922,18 +2057,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1962,16 +2085,16 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2404,14 +2527,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="39" t="s">
+      <c r="E3" s="53"/>
+      <c r="F3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="40"/>
+      <c r="G3" s="53"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -2434,16 +2557,16 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="45" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -2454,10 +2577,10 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
       <c r="F6" s="9" t="s">
         <v>29</v>
       </c>
@@ -2466,10 +2589,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="9" t="s">
         <v>31</v>
       </c>
@@ -2478,7 +2601,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="45" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -2498,14 +2621,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="42"/>
-      <c r="C9" s="41" t="s">
+      <c r="B9" s="46"/>
+      <c r="C9" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="43" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="12" t="s">
@@ -2516,10 +2639,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
       <c r="F10" s="12" t="s">
         <v>44</v>
       </c>
@@ -2528,7 +2651,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="45" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -2548,14 +2671,14 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="42"/>
-      <c r="C12" s="41" t="s">
+      <c r="B12" s="46"/>
+      <c r="C12" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="43" t="s">
         <v>52</v>
       </c>
       <c r="F12" s="12" t="s">
@@ -2566,10 +2689,10 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
       <c r="F13" s="12" t="s">
         <v>55</v>
       </c>
@@ -2578,7 +2701,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="45" t="s">
         <v>57</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -2598,14 +2721,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="42"/>
-      <c r="C15" s="41" t="s">
+      <c r="B15" s="46"/>
+      <c r="C15" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="44" t="s">
+      <c r="E15" s="43" t="s">
         <v>63</v>
       </c>
       <c r="F15" s="12" t="s">
@@ -2616,10 +2739,10 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
       <c r="F16" s="12" t="s">
         <v>66</v>
       </c>
@@ -2628,7 +2751,7 @@
       </c>
     </row>
     <row r="17" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="43"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="9" t="s">
         <v>34</v>
       </c>
@@ -2642,7 +2765,7 @@
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="45" t="s">
         <v>70</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -2662,33 +2785,33 @@
       </c>
     </row>
     <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="42"/>
-      <c r="C19" s="41" t="s">
+      <c r="B19" s="46"/>
+      <c r="C19" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="44" t="s">
+      <c r="D19" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="44" t="s">
+      <c r="E19" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="44" t="s">
+      <c r="F19" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="44" t="s">
+      <c r="G19" s="43" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="42"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
     </row>
     <row r="21" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="43"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="9" t="s">
         <v>34</v>
       </c>
@@ -2702,16 +2825,16 @@
       <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="44" t="s">
+      <c r="D22" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="44" t="s">
+      <c r="E22" s="43" t="s">
         <v>83</v>
       </c>
       <c r="F22" s="11" t="s">
@@ -2723,17 +2846,17 @@
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="48"/>
-      <c r="O22" s="47"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="55"/>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
       <c r="F23" s="12" t="s">
         <v>86</v>
       </c>
@@ -2750,10 +2873,10 @@
       <c r="P23" s="4"/>
     </row>
     <row r="24" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
       <c r="F24" s="12" t="s">
         <v>88</v>
       </c>
@@ -2766,11 +2889,11 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="46"/>
+      <c r="O24" s="54"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="43"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="9" t="s">
         <v>34</v>
       </c>
@@ -2788,11 +2911,11 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="47"/>
+      <c r="O25" s="55"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="45" t="s">
         <v>91</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -2816,18 +2939,18 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="46"/>
+      <c r="O26" s="54"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="42"/>
-      <c r="C27" s="41" t="s">
+      <c r="B27" s="46"/>
+      <c r="C27" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="44" t="s">
+      <c r="D27" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="E27" s="44" t="s">
+      <c r="E27" s="43" t="s">
         <v>97</v>
       </c>
       <c r="F27" s="12" t="s">
@@ -2842,14 +2965,14 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="47"/>
+      <c r="O27" s="55"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="42"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
       <c r="F28" s="12" t="s">
         <v>100</v>
       </c>
@@ -2862,11 +2985,11 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="46"/>
+      <c r="O28" s="54"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="43"/>
+      <c r="B29" s="47"/>
       <c r="C29" s="9" t="s">
         <v>34</v>
       </c>
@@ -2884,11 +3007,11 @@
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="47"/>
+      <c r="O29" s="55"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="45" t="s">
         <v>103</v>
       </c>
       <c r="C30" s="10" t="s">
@@ -2916,14 +3039,14 @@
       <c r="P30" s="4"/>
     </row>
     <row r="31" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="42"/>
-      <c r="C31" s="41" t="s">
+      <c r="B31" s="46"/>
+      <c r="C31" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="44" t="s">
+      <c r="D31" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="44" t="s">
+      <c r="E31" s="43" t="s">
         <v>109</v>
       </c>
       <c r="F31" s="12" t="s">
@@ -2942,10 +3065,10 @@
       <c r="P31" s="4"/>
     </row>
     <row r="32" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="42"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
       <c r="F32" s="12" t="s">
         <v>112</v>
       </c>
@@ -2962,7 +3085,7 @@
       <c r="P32" s="4"/>
     </row>
     <row r="33" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="43"/>
+      <c r="B33" s="47"/>
       <c r="C33" s="9" t="s">
         <v>34</v>
       </c>
@@ -2984,10 +3107,10 @@
       <c r="P33" s="4"/>
     </row>
     <row r="34" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="41" t="s">
+      <c r="B34" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="45" t="s">
         <v>116</v>
       </c>
       <c r="D34" s="11" t="s">
@@ -2996,8 +3119,8 @@
       <c r="E34" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -3008,16 +3131,16 @@
       <c r="P34" s="4"/>
     </row>
     <row r="35" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
       <c r="D35" s="12" t="s">
         <v>119</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -3028,16 +3151,16 @@
       <c r="P35" s="4"/>
     </row>
     <row r="36" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="47"/>
       <c r="D36" s="12" t="s">
         <v>121</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -4033,6 +4156,35 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="O26:O27"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="C34:C36"/>
@@ -4049,35 +4201,6 @@
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="E22:E24"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -4090,7 +4213,7 @@
   <dimension ref="A1:S991"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4111,27 +4234,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="63" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="13"/>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="62"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="66"/>
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
@@ -4180,16 +4303,16 @@
       <c r="M3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="60" t="s">
+      <c r="N3" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="61"/>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="60" t="s">
+      <c r="O3" s="65"/>
+      <c r="P3" s="66"/>
+      <c r="Q3" s="64" t="s">
         <v>125</v>
       </c>
-      <c r="R3" s="61"/>
-      <c r="S3" s="62"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="66"/>
     </row>
     <row r="4" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
@@ -4231,16 +4354,16 @@
       <c r="M4" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="N4" s="56" t="s">
+      <c r="N4" s="60" t="s">
         <v>136</v>
       </c>
-      <c r="O4" s="57"/>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="56" t="s">
+      <c r="O4" s="61"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="R4" s="57"/>
-      <c r="S4" s="58"/>
+      <c r="R4" s="61"/>
+      <c r="S4" s="62"/>
     </row>
     <row r="5" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
@@ -4282,16 +4405,16 @@
       <c r="M5" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="N5" s="56" t="s">
+      <c r="N5" s="60" t="s">
         <v>136</v>
       </c>
-      <c r="O5" s="57"/>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="56" t="s">
+      <c r="O5" s="61"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="R5" s="57"/>
-      <c r="S5" s="58"/>
+      <c r="R5" s="61"/>
+      <c r="S5" s="62"/>
     </row>
     <row r="6" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
@@ -4333,16 +4456,16 @@
       <c r="M6" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="N6" s="56" t="s">
+      <c r="N6" s="60" t="s">
         <v>151</v>
       </c>
-      <c r="O6" s="57"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="56" t="s">
+      <c r="O6" s="61"/>
+      <c r="P6" s="62"/>
+      <c r="Q6" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="R6" s="57"/>
-      <c r="S6" s="58"/>
+      <c r="R6" s="61"/>
+      <c r="S6" s="62"/>
     </row>
     <row r="7" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -4384,16 +4507,16 @@
       <c r="M7" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="N7" s="56" t="s">
+      <c r="N7" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="O7" s="57"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="56" t="s">
+      <c r="O7" s="61"/>
+      <c r="P7" s="62"/>
+      <c r="Q7" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="R7" s="57"/>
-      <c r="S7" s="58"/>
+      <c r="R7" s="61"/>
+      <c r="S7" s="62"/>
     </row>
     <row r="8" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -4435,16 +4558,16 @@
       <c r="M8" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="N8" s="56" t="s">
+      <c r="N8" s="60" t="s">
         <v>167</v>
       </c>
-      <c r="O8" s="57"/>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="56" t="s">
+      <c r="O8" s="61"/>
+      <c r="P8" s="62"/>
+      <c r="Q8" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="R8" s="57"/>
-      <c r="S8" s="58"/>
+      <c r="R8" s="61"/>
+      <c r="S8" s="62"/>
     </row>
     <row r="9" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
@@ -4486,16 +4609,16 @@
       <c r="M9" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="N9" s="53" t="s">
+      <c r="N9" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="O9" s="54"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="56" t="s">
+      <c r="O9" s="58"/>
+      <c r="P9" s="59"/>
+      <c r="Q9" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="R9" s="57"/>
-      <c r="S9" s="58"/>
+      <c r="R9" s="61"/>
+      <c r="S9" s="62"/>
     </row>
     <row r="10" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
@@ -4537,16 +4660,16 @@
       <c r="M10" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="N10" s="53" t="s">
+      <c r="N10" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="O10" s="54"/>
-      <c r="P10" s="55"/>
-      <c r="Q10" s="56" t="s">
+      <c r="O10" s="58"/>
+      <c r="P10" s="59"/>
+      <c r="Q10" s="60" t="s">
         <v>183</v>
       </c>
-      <c r="R10" s="57"/>
-      <c r="S10" s="58"/>
+      <c r="R10" s="61"/>
+      <c r="S10" s="62"/>
     </row>
     <row r="11" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
@@ -4588,16 +4711,16 @@
       <c r="M11" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="N11" s="56" t="s">
+      <c r="N11" s="60" t="s">
         <v>191</v>
       </c>
-      <c r="O11" s="57"/>
-      <c r="P11" s="58"/>
-      <c r="Q11" s="56" t="s">
+      <c r="O11" s="61"/>
+      <c r="P11" s="62"/>
+      <c r="Q11" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="R11" s="57"/>
-      <c r="S11" s="58"/>
+      <c r="R11" s="61"/>
+      <c r="S11" s="62"/>
     </row>
     <row r="12" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
@@ -4639,16 +4762,16 @@
       <c r="M12" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="N12" s="53" t="s">
+      <c r="N12" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="O12" s="54"/>
-      <c r="P12" s="55"/>
-      <c r="Q12" s="56" t="s">
+      <c r="O12" s="58"/>
+      <c r="P12" s="59"/>
+      <c r="Q12" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="R12" s="57"/>
-      <c r="S12" s="58"/>
+      <c r="R12" s="61"/>
+      <c r="S12" s="62"/>
     </row>
     <row r="13" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
@@ -4690,16 +4813,16 @@
       <c r="M13" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="N13" s="53" t="s">
+      <c r="N13" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="O13" s="54"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="56" t="s">
+      <c r="O13" s="58"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="60" t="s">
         <v>205</v>
       </c>
-      <c r="R13" s="57"/>
-      <c r="S13" s="58"/>
+      <c r="R13" s="61"/>
+      <c r="S13" s="62"/>
     </row>
     <row r="14" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
@@ -4741,16 +4864,16 @@
       <c r="M14" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="N14" s="56" t="s">
+      <c r="N14" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="O14" s="57"/>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="56" t="s">
+      <c r="O14" s="61"/>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="R14" s="57"/>
-      <c r="S14" s="58"/>
+      <c r="R14" s="61"/>
+      <c r="S14" s="62"/>
     </row>
     <row r="15" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
@@ -4792,16 +4915,16 @@
       <c r="M15" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="N15" s="53" t="s">
+      <c r="N15" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="O15" s="54"/>
-      <c r="P15" s="55"/>
-      <c r="Q15" s="56" t="s">
+      <c r="O15" s="58"/>
+      <c r="P15" s="59"/>
+      <c r="Q15" s="60" t="s">
         <v>219</v>
       </c>
-      <c r="R15" s="57"/>
-      <c r="S15" s="58"/>
+      <c r="R15" s="61"/>
+      <c r="S15" s="62"/>
     </row>
     <row r="16" spans="1:19" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
@@ -4843,16 +4966,16 @@
       <c r="M16" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="N16" s="53" t="s">
+      <c r="N16" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="O16" s="54"/>
-      <c r="P16" s="55"/>
-      <c r="Q16" s="56" t="s">
+      <c r="O16" s="58"/>
+      <c r="P16" s="59"/>
+      <c r="Q16" s="60" t="s">
         <v>228</v>
       </c>
-      <c r="R16" s="57"/>
-      <c r="S16" s="58"/>
+      <c r="R16" s="61"/>
+      <c r="S16" s="62"/>
     </row>
     <row r="17" spans="1:19" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
@@ -4894,122 +5017,272 @@
       <c r="M17" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="N17" s="56" t="s">
+      <c r="N17" s="60" t="s">
         <v>234</v>
       </c>
-      <c r="O17" s="57"/>
-      <c r="P17" s="58"/>
-      <c r="Q17" s="56" t="s">
+      <c r="O17" s="61"/>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="R17" s="57"/>
-      <c r="S17" s="58"/>
+      <c r="R17" s="61"/>
+      <c r="S17" s="62"/>
     </row>
     <row r="18" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="39" t="s">
         <v>235</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="40" t="s">
         <v>236</v>
       </c>
-      <c r="C18" s="64" t="s">
+      <c r="C18" s="40" t="s">
         <v>237</v>
       </c>
-      <c r="D18" s="64">
+      <c r="D18" s="40">
         <v>7</v>
       </c>
-      <c r="E18" s="64" t="s">
+      <c r="E18" s="40" t="s">
         <v>238</v>
       </c>
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="40" t="s">
         <v>215</v>
       </c>
-      <c r="G18" s="64" t="s">
+      <c r="G18" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="H18" s="64">
+      <c r="H18" s="40">
         <v>5</v>
       </c>
-      <c r="I18" s="64" t="s">
+      <c r="I18" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="J18" s="64" t="s">
+      <c r="J18" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="K18" s="64" t="s">
+      <c r="K18" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="L18" s="64" t="s">
+      <c r="L18" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="M18" s="64" t="s">
+      <c r="M18" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="N18" s="53" t="s">
+      <c r="N18" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="O18" s="54"/>
-      <c r="P18" s="55"/>
-      <c r="Q18" s="56" t="s">
+      <c r="O18" s="58"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="60" t="s">
         <v>239</v>
       </c>
-      <c r="R18" s="57"/>
-      <c r="S18" s="58"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="62"/>
     </row>
     <row r="19" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="41" t="s">
         <v>240</v>
       </c>
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="42" t="s">
         <v>236</v>
       </c>
-      <c r="C19" s="66" t="s">
+      <c r="C19" s="42" t="s">
         <v>241</v>
       </c>
-      <c r="D19" s="66">
+      <c r="D19" s="42">
         <v>8</v>
       </c>
-      <c r="E19" s="66" t="s">
+      <c r="E19" s="42" t="s">
         <v>242</v>
       </c>
-      <c r="F19" s="66" t="s">
+      <c r="F19" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="G19" s="66" t="s">
+      <c r="G19" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="H19" s="66" t="s">
+      <c r="H19" s="42" t="s">
         <v>244</v>
       </c>
-      <c r="I19" s="66" t="s">
+      <c r="I19" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="J19" s="66" t="s">
+      <c r="J19" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="K19" s="66" t="s">
+      <c r="K19" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="L19" s="66" t="s">
+      <c r="L19" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="M19" s="66" t="s">
+      <c r="M19" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="N19" s="56" t="s">
+      <c r="N19" s="60" t="s">
         <v>245</v>
       </c>
-      <c r="O19" s="57"/>
-      <c r="P19" s="58"/>
-      <c r="Q19" s="56" t="s">
+      <c r="O19" s="61"/>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="R19" s="57"/>
-      <c r="S19" s="58"/>
+      <c r="R19" s="61"/>
+      <c r="S19" s="62"/>
     </row>
-    <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="67" t="s">
+        <v>246</v>
+      </c>
+      <c r="B20" s="68" t="s">
+        <v>247</v>
+      </c>
+      <c r="C20" s="68" t="s">
+        <v>248</v>
+      </c>
+      <c r="D20" s="68">
+        <v>42</v>
+      </c>
+      <c r="E20" s="68" t="s">
+        <v>249</v>
+      </c>
+      <c r="F20" s="68" t="s">
+        <v>232</v>
+      </c>
+      <c r="G20" s="68" t="s">
+        <v>134</v>
+      </c>
+      <c r="H20" s="68" t="s">
+        <v>134</v>
+      </c>
+      <c r="I20" s="68" t="s">
+        <v>156</v>
+      </c>
+      <c r="J20" s="68" t="s">
+        <v>134</v>
+      </c>
+      <c r="K20" s="68" t="s">
+        <v>134</v>
+      </c>
+      <c r="L20" s="68" t="s">
+        <v>134</v>
+      </c>
+      <c r="M20" s="68" t="s">
+        <v>150</v>
+      </c>
+      <c r="N20" s="60" t="s">
+        <v>250</v>
+      </c>
+      <c r="O20" s="61"/>
+      <c r="P20" s="62"/>
+      <c r="Q20" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="R20" s="61"/>
+      <c r="S20" s="62"/>
+    </row>
+    <row r="21" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="69" t="s">
+        <v>251</v>
+      </c>
+      <c r="B21" s="70" t="s">
+        <v>247</v>
+      </c>
+      <c r="C21" s="70" t="s">
+        <v>252</v>
+      </c>
+      <c r="D21" s="70">
+        <v>4</v>
+      </c>
+      <c r="E21" s="70" t="s">
+        <v>253</v>
+      </c>
+      <c r="F21" s="70" t="s">
+        <v>254</v>
+      </c>
+      <c r="G21" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="H21" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="I21" s="70">
+        <v>0</v>
+      </c>
+      <c r="J21" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="K21" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="L21" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="M21" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="N21" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="O21" s="58"/>
+      <c r="P21" s="59"/>
+      <c r="Q21" s="60" t="s">
+        <v>255</v>
+      </c>
+      <c r="R21" s="61"/>
+      <c r="S21" s="62"/>
+    </row>
+    <row r="22" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="69" t="s">
+        <v>256</v>
+      </c>
+      <c r="B22" s="70" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" s="70" t="s">
+        <v>257</v>
+      </c>
+      <c r="D22" s="70">
+        <v>5</v>
+      </c>
+      <c r="E22" s="70" t="s">
+        <v>258</v>
+      </c>
+      <c r="F22" s="70" t="s">
+        <v>259</v>
+      </c>
+      <c r="G22" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="H22" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="I22" s="70">
+        <v>5225</v>
+      </c>
+      <c r="J22" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="K22" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="L22" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="M22" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="N22" s="60" t="s">
+        <v>260</v>
+      </c>
+      <c r="O22" s="61"/>
+      <c r="P22" s="62"/>
+      <c r="Q22" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="R22" s="61"/>
+      <c r="S22" s="62"/>
+    </row>
     <row r="23" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5980,23 +6253,13 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
+  <mergeCells count="42">
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="Q22:S22"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="Q11:S11"/>
     <mergeCell ref="N5:P5"/>
@@ -6011,6 +6274,22 @@
     <mergeCell ref="Q7:S7"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="Q14:S14"/>
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="Q15:S15"/>
     <mergeCell ref="N16:P16"/>

</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas Distrito incorrectas se reporta errores en el CP20 y CP21
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60548168-D88A-4DC1-8C9A-FAFD38A81FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF03407-0480-4E1C-940B-839070AC75C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="280">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -1520,6 +1520,123 @@
   </si>
   <si>
     <t>No se permite el ingreso de "5225" como Lote</t>
+  </si>
+  <si>
+    <t>CP20</t>
+  </si>
+  <si>
+    <t>Registro con Distrito Incorrecto</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;08&gt; ,CEV&lt;11&gt; ,CEV&lt;16&gt; ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> CENV&lt;18&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> CEV&lt;19&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Ríos</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>5187*/</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir números y carácteres no alfanuméricos como Distrito</t>
+  </si>
+  <si>
+    <t>CP21</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;08&gt; ,CEV&lt;11&gt; ,CEV&lt;16&gt; ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;19&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, CEV&lt;19&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Silva</t>
+  </si>
+  <si>
+    <t>Nina</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir Distrito de una letra</t>
+  </si>
+  <si>
+    <t>CP22</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;08&gt; ,CEV&lt;11&gt; ,CEV&lt;16&gt; ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;20&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> , CEV&lt;19&gt; , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Mendoza</t>
+  </si>
+  <si>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t>dsafdsfewfewgewrgerwgregeryhgfghjgfjfgjgfjgfjtyjygjykjhyutkyk8yulyutktykytktykkytky</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "dsafdsfewfewgewrge,,,,," como Distrito</t>
   </si>
 </sst>
 </file>
@@ -2019,12 +2136,22 @@
     <xf numFmtId="0" fontId="10" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2033,6 +2160,19 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2046,16 +2186,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2066,15 +2204,6 @@
     <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2083,18 +2212,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2527,14 +2644,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="53"/>
-      <c r="F3" s="52" t="s">
+      <c r="E3" s="48"/>
+      <c r="F3" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="53"/>
+      <c r="G3" s="48"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -2557,16 +2674,16 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="49" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -2577,10 +2694,10 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
       <c r="F6" s="9" t="s">
         <v>29</v>
       </c>
@@ -2589,10 +2706,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="9" t="s">
         <v>31</v>
       </c>
@@ -2601,7 +2718,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="49" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -2621,14 +2738,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46"/>
-      <c r="C9" s="45" t="s">
+      <c r="B9" s="50"/>
+      <c r="C9" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="52" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="12" t="s">
@@ -2639,10 +2756,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
       <c r="F10" s="12" t="s">
         <v>44</v>
       </c>
@@ -2651,7 +2768,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="49" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -2671,14 +2788,14 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46"/>
-      <c r="C12" s="45" t="s">
+      <c r="B12" s="50"/>
+      <c r="C12" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="52" t="s">
         <v>52</v>
       </c>
       <c r="F12" s="12" t="s">
@@ -2689,10 +2806,10 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
       <c r="F13" s="12" t="s">
         <v>55</v>
       </c>
@@ -2701,7 +2818,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="49" t="s">
         <v>57</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -2721,14 +2838,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="46"/>
-      <c r="C15" s="45" t="s">
+      <c r="B15" s="50"/>
+      <c r="C15" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="52" t="s">
         <v>63</v>
       </c>
       <c r="F15" s="12" t="s">
@@ -2739,10 +2856,10 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="46"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
       <c r="F16" s="12" t="s">
         <v>66</v>
       </c>
@@ -2751,7 +2868,7 @@
       </c>
     </row>
     <row r="17" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="9" t="s">
         <v>34</v>
       </c>
@@ -2765,7 +2882,7 @@
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="49" t="s">
         <v>70</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -2785,33 +2902,33 @@
       </c>
     </row>
     <row r="19" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="46"/>
-      <c r="C19" s="45" t="s">
+      <c r="B19" s="50"/>
+      <c r="C19" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="43" t="s">
+      <c r="F19" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="43" t="s">
+      <c r="G19" s="52" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="46"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
     </row>
     <row r="21" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="47"/>
+      <c r="B21" s="51"/>
       <c r="C21" s="9" t="s">
         <v>34</v>
       </c>
@@ -2825,16 +2942,16 @@
       <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="43" t="s">
+      <c r="D22" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="52" t="s">
         <v>83</v>
       </c>
       <c r="F22" s="11" t="s">
@@ -2853,10 +2970,10 @@
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
       <c r="F23" s="12" t="s">
         <v>86</v>
       </c>
@@ -2873,10 +2990,10 @@
       <c r="P23" s="4"/>
     </row>
     <row r="24" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
       <c r="F24" s="12" t="s">
         <v>88</v>
       </c>
@@ -2893,7 +3010,7 @@
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
+      <c r="B25" s="51"/>
       <c r="C25" s="9" t="s">
         <v>34</v>
       </c>
@@ -2915,7 +3032,7 @@
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="49" t="s">
         <v>91</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -2943,14 +3060,14 @@
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="46"/>
-      <c r="C27" s="45" t="s">
+      <c r="B27" s="50"/>
+      <c r="C27" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="43" t="s">
+      <c r="D27" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E27" s="52" t="s">
         <v>97</v>
       </c>
       <c r="F27" s="12" t="s">
@@ -2969,10 +3086,10 @@
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="46"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
       <c r="F28" s="12" t="s">
         <v>100</v>
       </c>
@@ -2989,7 +3106,7 @@
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="47"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="9" t="s">
         <v>34</v>
       </c>
@@ -3011,7 +3128,7 @@
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="45" t="s">
+      <c r="B30" s="49" t="s">
         <v>103</v>
       </c>
       <c r="C30" s="10" t="s">
@@ -3039,14 +3156,14 @@
       <c r="P30" s="4"/>
     </row>
     <row r="31" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="46"/>
-      <c r="C31" s="45" t="s">
+      <c r="B31" s="50"/>
+      <c r="C31" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="43" t="s">
+      <c r="D31" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="43" t="s">
+      <c r="E31" s="52" t="s">
         <v>109</v>
       </c>
       <c r="F31" s="12" t="s">
@@ -3065,10 +3182,10 @@
       <c r="P31" s="4"/>
     </row>
     <row r="32" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="46"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
       <c r="F32" s="12" t="s">
         <v>112</v>
       </c>
@@ -3085,7 +3202,7 @@
       <c r="P32" s="4"/>
     </row>
     <row r="33" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="47"/>
+      <c r="B33" s="51"/>
       <c r="C33" s="9" t="s">
         <v>34</v>
       </c>
@@ -3107,10 +3224,10 @@
       <c r="P33" s="4"/>
     </row>
     <row r="34" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="C34" s="45" t="s">
+      <c r="C34" s="49" t="s">
         <v>116</v>
       </c>
       <c r="D34" s="11" t="s">
@@ -3119,8 +3236,8 @@
       <c r="E34" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -3131,16 +3248,16 @@
       <c r="P34" s="4"/>
     </row>
     <row r="35" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="46"/>
-      <c r="C35" s="46"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
       <c r="D35" s="12" t="s">
         <v>119</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -3151,16 +3268,16 @@
       <c r="P35" s="4"/>
     </row>
     <row r="36" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="47"/>
-      <c r="C36" s="47"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="51"/>
       <c r="D36" s="12" t="s">
         <v>121</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -4156,6 +4273,35 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="E27:E28"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C15:C16"/>
@@ -4172,35 +4318,6 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -4212,8 +4329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4234,7 +4351,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="67" t="s">
         <v>123</v>
       </c>
       <c r="B1" s="55"/>
@@ -4244,17 +4361,17 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="13"/>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="66"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="70"/>
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
@@ -4303,16 +4420,16 @@
       <c r="M3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="64" t="s">
+      <c r="N3" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="65"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="64" t="s">
+      <c r="O3" s="69"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="R3" s="65"/>
-      <c r="S3" s="66"/>
+      <c r="R3" s="69"/>
+      <c r="S3" s="70"/>
     </row>
     <row r="4" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
@@ -4354,16 +4471,16 @@
       <c r="M4" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="N4" s="60" t="s">
+      <c r="N4" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="O4" s="61"/>
-      <c r="P4" s="62"/>
-      <c r="Q4" s="60" t="s">
+      <c r="O4" s="62"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="R4" s="61"/>
-      <c r="S4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="63"/>
     </row>
     <row r="5" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
@@ -4405,16 +4522,16 @@
       <c r="M5" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="N5" s="60" t="s">
+      <c r="N5" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="60" t="s">
+      <c r="O5" s="62"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="R5" s="61"/>
-      <c r="S5" s="62"/>
+      <c r="R5" s="62"/>
+      <c r="S5" s="63"/>
     </row>
     <row r="6" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
@@ -4456,16 +4573,16 @@
       <c r="M6" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="N6" s="60" t="s">
+      <c r="N6" s="61" t="s">
         <v>151</v>
       </c>
-      <c r="O6" s="61"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="60" t="s">
+      <c r="O6" s="62"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="R6" s="61"/>
-      <c r="S6" s="62"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="63"/>
     </row>
     <row r="7" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -4507,16 +4624,16 @@
       <c r="M7" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="N7" s="60" t="s">
+      <c r="N7" s="61" t="s">
         <v>159</v>
       </c>
-      <c r="O7" s="61"/>
-      <c r="P7" s="62"/>
-      <c r="Q7" s="60" t="s">
+      <c r="O7" s="62"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="R7" s="61"/>
-      <c r="S7" s="62"/>
+      <c r="R7" s="62"/>
+      <c r="S7" s="63"/>
     </row>
     <row r="8" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -4558,16 +4675,16 @@
       <c r="M8" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="N8" s="60" t="s">
+      <c r="N8" s="61" t="s">
         <v>167</v>
       </c>
-      <c r="O8" s="61"/>
-      <c r="P8" s="62"/>
-      <c r="Q8" s="60" t="s">
+      <c r="O8" s="62"/>
+      <c r="P8" s="63"/>
+      <c r="Q8" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="R8" s="61"/>
-      <c r="S8" s="62"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="63"/>
     </row>
     <row r="9" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
@@ -4609,16 +4726,16 @@
       <c r="M9" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="N9" s="57" t="s">
+      <c r="N9" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="O9" s="58"/>
-      <c r="P9" s="59"/>
-      <c r="Q9" s="60" t="s">
+      <c r="O9" s="65"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R9" s="61"/>
-      <c r="S9" s="62"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="63"/>
     </row>
     <row r="10" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
@@ -4660,16 +4777,16 @@
       <c r="M10" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="N10" s="57" t="s">
+      <c r="N10" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="O10" s="58"/>
-      <c r="P10" s="59"/>
-      <c r="Q10" s="60" t="s">
+      <c r="O10" s="65"/>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="61" t="s">
         <v>183</v>
       </c>
-      <c r="R10" s="61"/>
-      <c r="S10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="63"/>
     </row>
     <row r="11" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
@@ -4711,16 +4828,16 @@
       <c r="M11" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="N11" s="60" t="s">
+      <c r="N11" s="61" t="s">
         <v>191</v>
       </c>
-      <c r="O11" s="61"/>
-      <c r="P11" s="62"/>
-      <c r="Q11" s="60" t="s">
+      <c r="O11" s="62"/>
+      <c r="P11" s="63"/>
+      <c r="Q11" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="R11" s="61"/>
-      <c r="S11" s="62"/>
+      <c r="R11" s="62"/>
+      <c r="S11" s="63"/>
     </row>
     <row r="12" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
@@ -4762,16 +4879,16 @@
       <c r="M12" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="N12" s="57" t="s">
+      <c r="N12" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="O12" s="58"/>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="60" t="s">
+      <c r="O12" s="65"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="R12" s="61"/>
-      <c r="S12" s="62"/>
+      <c r="R12" s="62"/>
+      <c r="S12" s="63"/>
     </row>
     <row r="13" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
@@ -4813,16 +4930,16 @@
       <c r="M13" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="N13" s="57" t="s">
+      <c r="N13" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="O13" s="58"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="60" t="s">
+      <c r="O13" s="65"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="61" t="s">
         <v>205</v>
       </c>
-      <c r="R13" s="61"/>
-      <c r="S13" s="62"/>
+      <c r="R13" s="62"/>
+      <c r="S13" s="63"/>
     </row>
     <row r="14" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
@@ -4864,16 +4981,16 @@
       <c r="M14" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="N14" s="60" t="s">
+      <c r="N14" s="61" t="s">
         <v>211</v>
       </c>
-      <c r="O14" s="61"/>
-      <c r="P14" s="62"/>
-      <c r="Q14" s="60" t="s">
+      <c r="O14" s="62"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="R14" s="61"/>
-      <c r="S14" s="62"/>
+      <c r="R14" s="62"/>
+      <c r="S14" s="63"/>
     </row>
     <row r="15" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
@@ -4915,16 +5032,16 @@
       <c r="M15" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="N15" s="57" t="s">
+      <c r="N15" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="O15" s="58"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="60" t="s">
+      <c r="O15" s="65"/>
+      <c r="P15" s="66"/>
+      <c r="Q15" s="61" t="s">
         <v>219</v>
       </c>
-      <c r="R15" s="61"/>
-      <c r="S15" s="62"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="63"/>
     </row>
     <row r="16" spans="1:19" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
@@ -4966,16 +5083,16 @@
       <c r="M16" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="N16" s="57" t="s">
+      <c r="N16" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="O16" s="58"/>
-      <c r="P16" s="59"/>
-      <c r="Q16" s="60" t="s">
+      <c r="O16" s="65"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="61" t="s">
         <v>228</v>
       </c>
-      <c r="R16" s="61"/>
-      <c r="S16" s="62"/>
+      <c r="R16" s="62"/>
+      <c r="S16" s="63"/>
     </row>
     <row r="17" spans="1:19" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
@@ -5017,16 +5134,16 @@
       <c r="M17" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="N17" s="60" t="s">
+      <c r="N17" s="61" t="s">
         <v>234</v>
       </c>
-      <c r="O17" s="61"/>
-      <c r="P17" s="62"/>
-      <c r="Q17" s="60" t="s">
+      <c r="O17" s="62"/>
+      <c r="P17" s="63"/>
+      <c r="Q17" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="R17" s="61"/>
-      <c r="S17" s="62"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="63"/>
     </row>
     <row r="18" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="39" t="s">
@@ -5068,16 +5185,16 @@
       <c r="M18" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="N18" s="57" t="s">
+      <c r="N18" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="O18" s="58"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="60" t="s">
+      <c r="O18" s="65"/>
+      <c r="P18" s="66"/>
+      <c r="Q18" s="61" t="s">
         <v>239</v>
       </c>
-      <c r="R18" s="61"/>
-      <c r="S18" s="62"/>
+      <c r="R18" s="62"/>
+      <c r="S18" s="63"/>
     </row>
     <row r="19" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="41" t="s">
@@ -5119,173 +5236,323 @@
       <c r="M19" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="N19" s="60" t="s">
+      <c r="N19" s="61" t="s">
         <v>245</v>
       </c>
-      <c r="O19" s="61"/>
-      <c r="P19" s="62"/>
-      <c r="Q19" s="60" t="s">
+      <c r="O19" s="62"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="R19" s="61"/>
-      <c r="S19" s="62"/>
+      <c r="R19" s="62"/>
+      <c r="S19" s="63"/>
     </row>
     <row r="20" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="43" t="s">
         <v>246</v>
       </c>
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="44" t="s">
         <v>247</v>
       </c>
-      <c r="C20" s="68" t="s">
+      <c r="C20" s="44" t="s">
         <v>248</v>
       </c>
-      <c r="D20" s="68">
+      <c r="D20" s="44">
         <v>42</v>
       </c>
-      <c r="E20" s="68" t="s">
+      <c r="E20" s="44" t="s">
         <v>249</v>
       </c>
-      <c r="F20" s="68" t="s">
+      <c r="F20" s="44" t="s">
         <v>232</v>
       </c>
-      <c r="G20" s="68" t="s">
+      <c r="G20" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="H20" s="68" t="s">
+      <c r="H20" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="I20" s="68" t="s">
+      <c r="I20" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="J20" s="68" t="s">
+      <c r="J20" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="K20" s="68" t="s">
+      <c r="K20" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="L20" s="68" t="s">
+      <c r="L20" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="M20" s="68" t="s">
+      <c r="M20" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="N20" s="60" t="s">
+      <c r="N20" s="61" t="s">
         <v>250</v>
       </c>
-      <c r="O20" s="61"/>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="60" t="s">
+      <c r="O20" s="62"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="R20" s="61"/>
-      <c r="S20" s="62"/>
+      <c r="R20" s="62"/>
+      <c r="S20" s="63"/>
     </row>
     <row r="21" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="69" t="s">
+      <c r="A21" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="46" t="s">
         <v>247</v>
       </c>
-      <c r="C21" s="70" t="s">
+      <c r="C21" s="46" t="s">
         <v>252</v>
       </c>
-      <c r="D21" s="70">
+      <c r="D21" s="46">
         <v>4</v>
       </c>
-      <c r="E21" s="70" t="s">
+      <c r="E21" s="46" t="s">
         <v>253</v>
       </c>
-      <c r="F21" s="70" t="s">
+      <c r="F21" s="46" t="s">
         <v>254</v>
       </c>
-      <c r="G21" s="70" t="s">
+      <c r="G21" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="H21" s="70" t="s">
+      <c r="H21" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="I21" s="70">
+      <c r="I21" s="46">
         <v>0</v>
       </c>
-      <c r="J21" s="70" t="s">
+      <c r="J21" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="K21" s="70" t="s">
+      <c r="K21" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="L21" s="70" t="s">
+      <c r="L21" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="M21" s="70" t="s">
+      <c r="M21" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="N21" s="57" t="s">
+      <c r="N21" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="O21" s="58"/>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="60" t="s">
+      <c r="O21" s="65"/>
+      <c r="P21" s="66"/>
+      <c r="Q21" s="61" t="s">
         <v>255</v>
       </c>
-      <c r="R21" s="61"/>
-      <c r="S21" s="62"/>
+      <c r="R21" s="62"/>
+      <c r="S21" s="63"/>
     </row>
     <row r="22" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="69" t="s">
+      <c r="A22" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="B22" s="70" t="s">
+      <c r="B22" s="46" t="s">
         <v>247</v>
       </c>
-      <c r="C22" s="70" t="s">
+      <c r="C22" s="46" t="s">
         <v>257</v>
       </c>
-      <c r="D22" s="70">
+      <c r="D22" s="46">
         <v>5</v>
       </c>
-      <c r="E22" s="70" t="s">
+      <c r="E22" s="46" t="s">
         <v>258</v>
       </c>
-      <c r="F22" s="70" t="s">
+      <c r="F22" s="46" t="s">
         <v>259</v>
       </c>
-      <c r="G22" s="70" t="s">
+      <c r="G22" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="H22" s="70" t="s">
+      <c r="H22" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="I22" s="70">
+      <c r="I22" s="46">
         <v>5225</v>
       </c>
-      <c r="J22" s="70" t="s">
+      <c r="J22" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="K22" s="70" t="s">
+      <c r="K22" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="L22" s="70" t="s">
+      <c r="L22" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="M22" s="70" t="s">
+      <c r="M22" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="N22" s="60" t="s">
+      <c r="N22" s="61" t="s">
         <v>260</v>
       </c>
-      <c r="O22" s="61"/>
-      <c r="P22" s="62"/>
-      <c r="Q22" s="60" t="s">
+      <c r="O22" s="62"/>
+      <c r="P22" s="63"/>
+      <c r="Q22" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="R22" s="61"/>
-      <c r="S22" s="62"/>
+      <c r="R22" s="62"/>
+      <c r="S22" s="63"/>
     </row>
-    <row r="23" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="D23" s="28">
+        <v>68</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="I23" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="K23" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="L23" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="M23" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="N23" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="O23" s="65"/>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="61" t="s">
+        <v>267</v>
+      </c>
+      <c r="R23" s="62"/>
+      <c r="S23" s="63"/>
+    </row>
+    <row r="24" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>262</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>269</v>
+      </c>
+      <c r="D24" s="30">
+        <v>5</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>271</v>
+      </c>
+      <c r="G24" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="I24" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="J24" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="K24" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="L24" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="M24" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="N24" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="O24" s="65"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="61" t="s">
+        <v>273</v>
+      </c>
+      <c r="R24" s="62"/>
+      <c r="S24" s="63"/>
+    </row>
+    <row r="25" spans="1:19" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>262</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>275</v>
+      </c>
+      <c r="D25" s="30">
+        <v>9</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>276</v>
+      </c>
+      <c r="F25" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="G25" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="H25" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="I25" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="J25" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="K25" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="L25" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="M25" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="N25" s="61" t="s">
+        <v>279</v>
+      </c>
+      <c r="O25" s="62"/>
+      <c r="P25" s="63"/>
+      <c r="Q25" s="61" t="s">
+        <v>137</v>
+      </c>
+      <c r="R25" s="62"/>
+      <c r="S25" s="63"/>
+    </row>
     <row r="26" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6253,33 +6520,13 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
+  <mergeCells count="48">
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="Q25:S25"/>
     <mergeCell ref="N18:P18"/>
     <mergeCell ref="Q18:S18"/>
     <mergeCell ref="N19:P19"/>
@@ -6296,6 +6543,32 @@
     <mergeCell ref="Q16:S16"/>
     <mergeCell ref="N17:P17"/>
     <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="Q22:S22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas Provincia incorrectas se reporta errores en el CP23 y CP24
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF03407-0480-4E1C-940B-839070AC75C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19437B5D-4C22-4045-99FD-AF660133CC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clases de equialencia Nuevo U" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="299">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -1637,6 +1637,123 @@
   </si>
   <si>
     <t>No se permite el ingreso de "dsafdsfewfewgewrge,,,,," como Distrito</t>
+  </si>
+  <si>
+    <t>CP23</t>
+  </si>
+  <si>
+    <t>Registro con Provincia Incorrecto</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;08&gt; ,CEV&lt;11&gt; ,CEV&lt;16&gt; , CEV&lt;14&gt; ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;21&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Vargas</t>
+  </si>
+  <si>
+    <t>Maya</t>
+  </si>
+  <si>
+    <t>/*/84</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir números y carácteres no alfanuméricos como Provincia</t>
+  </si>
+  <si>
+    <t>CP24</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;08&gt; ,CEV&lt;11&gt; ,CEV&lt;16&gt; , CEV&lt;14&gt; ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;22&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> , CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Núñez</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>ñ</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir Provincia de una letra</t>
+  </si>
+  <si>
+    <t>CP25</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;08&gt; ,CEV&lt;11&gt; ,CEV&lt;16&gt; , CEV&lt;14&gt; ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> CENV&lt;23&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, CEV&lt;22&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Bravo</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>nkgdnkgrmkgrmkgrmkgrmklgrmg,mlfm,dhlm,rhmrlmlhmllfdlfdhlfhd</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "nkgdnkgrmkgrm,,,,," como Provincia</t>
   </si>
 </sst>
 </file>
@@ -1721,7 +1838,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1791,6 +1908,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD5A6BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2010,7 +2133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2148,25 +2271,37 @@
     <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2174,17 +2309,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2193,15 +2325,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2212,6 +2335,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2624,7 +2759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
@@ -2644,14 +2779,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="47" t="s">
+      <c r="E3" s="57"/>
+      <c r="F3" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="48"/>
+      <c r="G3" s="57"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -2742,10 +2877,10 @@
       <c r="C9" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E9" s="47" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="12" t="s">
@@ -2758,8 +2893,8 @@
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
       <c r="F10" s="12" t="s">
         <v>44</v>
       </c>
@@ -2792,10 +2927,10 @@
       <c r="C12" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="47" t="s">
         <v>52</v>
       </c>
       <c r="F12" s="12" t="s">
@@ -2808,8 +2943,8 @@
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="12" t="s">
         <v>55</v>
       </c>
@@ -2842,10 +2977,10 @@
       <c r="C15" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="47" t="s">
         <v>63</v>
       </c>
       <c r="F15" s="12" t="s">
@@ -2858,8 +2993,8 @@
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="50"/>
       <c r="C16" s="51"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
       <c r="F16" s="12" t="s">
         <v>66</v>
       </c>
@@ -2906,26 +3041,26 @@
       <c r="C19" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="52" t="s">
+      <c r="D19" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="52" t="s">
+      <c r="E19" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="52" t="s">
+      <c r="F19" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="52" t="s">
+      <c r="G19" s="47" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="50"/>
       <c r="C20" s="51"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
     </row>
     <row r="21" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="51"/>
@@ -2948,10 +3083,10 @@
       <c r="C22" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="52" t="s">
+      <c r="D22" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="52" t="s">
+      <c r="E22" s="47" t="s">
         <v>83</v>
       </c>
       <c r="F22" s="11" t="s">
@@ -2963,17 +3098,17 @@
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="55"/>
-      <c r="N22" s="56"/>
-      <c r="O22" s="55"/>
+      <c r="L22" s="60"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="60"/>
+      <c r="O22" s="59"/>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="50"/>
       <c r="C23" s="50"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
       <c r="F23" s="12" t="s">
         <v>86</v>
       </c>
@@ -2992,8 +3127,8 @@
     <row r="24" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="50"/>
       <c r="C24" s="51"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
       <c r="F24" s="12" t="s">
         <v>88</v>
       </c>
@@ -3006,7 +3141,7 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="54"/>
+      <c r="O24" s="58"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3028,7 +3163,7 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="55"/>
+      <c r="O25" s="59"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3056,7 +3191,7 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="54"/>
+      <c r="O26" s="58"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3064,10 +3199,10 @@
       <c r="C27" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="52" t="s">
+      <c r="D27" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="E27" s="52" t="s">
+      <c r="E27" s="47" t="s">
         <v>97</v>
       </c>
       <c r="F27" s="12" t="s">
@@ -3082,14 +3217,14 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="55"/>
+      <c r="O27" s="59"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="50"/>
       <c r="C28" s="51"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
       <c r="F28" s="12" t="s">
         <v>100</v>
       </c>
@@ -3102,7 +3237,7 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="54"/>
+      <c r="O28" s="58"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3124,7 +3259,7 @@
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="55"/>
+      <c r="O29" s="59"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3160,10 +3295,10 @@
       <c r="C31" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="52" t="s">
+      <c r="D31" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="52" t="s">
+      <c r="E31" s="47" t="s">
         <v>109</v>
       </c>
       <c r="F31" s="12" t="s">
@@ -3184,8 +3319,8 @@
     <row r="32" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="50"/>
       <c r="C32" s="51"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
       <c r="F32" s="12" t="s">
         <v>112</v>
       </c>
@@ -3236,8 +3371,8 @@
       <c r="E34" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -3256,8 +3391,8 @@
       <c r="E35" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -3276,8 +3411,8 @@
       <c r="E36" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="54"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -4273,6 +4408,35 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="O26:O27"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="C34:C36"/>
@@ -4289,35 +4453,6 @@
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="E22:E24"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -4329,8 +4464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S991"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4344,9 +4479,10 @@
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="19.5703125" customWidth="1"/>
-    <col min="10" max="11" width="10" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
     <col min="14" max="28" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4354,8 +4490,8 @@
       <c r="A1" s="67" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
@@ -4471,16 +4607,16 @@
       <c r="M4" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="N4" s="61" t="s">
+      <c r="N4" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="O4" s="62"/>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="61" t="s">
+      <c r="O4" s="65"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="R4" s="62"/>
-      <c r="S4" s="63"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="66"/>
     </row>
     <row r="5" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
@@ -4522,16 +4658,16 @@
       <c r="M5" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="N5" s="61" t="s">
+      <c r="N5" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="O5" s="62"/>
-      <c r="P5" s="63"/>
-      <c r="Q5" s="61" t="s">
+      <c r="O5" s="65"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="R5" s="62"/>
-      <c r="S5" s="63"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="66"/>
     </row>
     <row r="6" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
@@ -4573,16 +4709,16 @@
       <c r="M6" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="N6" s="61" t="s">
+      <c r="N6" s="64" t="s">
         <v>151</v>
       </c>
-      <c r="O6" s="62"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="61" t="s">
+      <c r="O6" s="65"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="R6" s="62"/>
-      <c r="S6" s="63"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="66"/>
     </row>
     <row r="7" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -4624,16 +4760,16 @@
       <c r="M7" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="N7" s="61" t="s">
+      <c r="N7" s="64" t="s">
         <v>159</v>
       </c>
-      <c r="O7" s="62"/>
-      <c r="P7" s="63"/>
-      <c r="Q7" s="61" t="s">
+      <c r="O7" s="65"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="R7" s="62"/>
-      <c r="S7" s="63"/>
+      <c r="R7" s="65"/>
+      <c r="S7" s="66"/>
     </row>
     <row r="8" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -4675,16 +4811,16 @@
       <c r="M8" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="N8" s="61" t="s">
+      <c r="N8" s="64" t="s">
         <v>167</v>
       </c>
-      <c r="O8" s="62"/>
-      <c r="P8" s="63"/>
-      <c r="Q8" s="61" t="s">
+      <c r="O8" s="65"/>
+      <c r="P8" s="66"/>
+      <c r="Q8" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="R8" s="62"/>
-      <c r="S8" s="63"/>
+      <c r="R8" s="65"/>
+      <c r="S8" s="66"/>
     </row>
     <row r="9" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
@@ -4726,16 +4862,16 @@
       <c r="M9" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="N9" s="64" t="s">
+      <c r="N9" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="O9" s="65"/>
-      <c r="P9" s="66"/>
-      <c r="Q9" s="61" t="s">
+      <c r="O9" s="62"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="64" t="s">
         <v>175</v>
       </c>
-      <c r="R9" s="62"/>
-      <c r="S9" s="63"/>
+      <c r="R9" s="65"/>
+      <c r="S9" s="66"/>
     </row>
     <row r="10" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
@@ -4777,16 +4913,16 @@
       <c r="M10" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="N10" s="64" t="s">
+      <c r="N10" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="O10" s="65"/>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="61" t="s">
+      <c r="O10" s="62"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="64" t="s">
         <v>183</v>
       </c>
-      <c r="R10" s="62"/>
-      <c r="S10" s="63"/>
+      <c r="R10" s="65"/>
+      <c r="S10" s="66"/>
     </row>
     <row r="11" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
@@ -4828,16 +4964,16 @@
       <c r="M11" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="N11" s="61" t="s">
+      <c r="N11" s="64" t="s">
         <v>191</v>
       </c>
-      <c r="O11" s="62"/>
-      <c r="P11" s="63"/>
-      <c r="Q11" s="61" t="s">
+      <c r="O11" s="65"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="R11" s="62"/>
-      <c r="S11" s="63"/>
+      <c r="R11" s="65"/>
+      <c r="S11" s="66"/>
     </row>
     <row r="12" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
@@ -4879,16 +5015,16 @@
       <c r="M12" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="N12" s="64" t="s">
+      <c r="N12" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="O12" s="65"/>
-      <c r="P12" s="66"/>
-      <c r="Q12" s="61" t="s">
+      <c r="O12" s="62"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="64" t="s">
         <v>197</v>
       </c>
-      <c r="R12" s="62"/>
-      <c r="S12" s="63"/>
+      <c r="R12" s="65"/>
+      <c r="S12" s="66"/>
     </row>
     <row r="13" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
@@ -4930,16 +5066,16 @@
       <c r="M13" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="N13" s="64" t="s">
+      <c r="N13" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="O13" s="65"/>
-      <c r="P13" s="66"/>
-      <c r="Q13" s="61" t="s">
+      <c r="O13" s="62"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="64" t="s">
         <v>205</v>
       </c>
-      <c r="R13" s="62"/>
-      <c r="S13" s="63"/>
+      <c r="R13" s="65"/>
+      <c r="S13" s="66"/>
     </row>
     <row r="14" spans="1:19" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
@@ -4981,16 +5117,16 @@
       <c r="M14" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="N14" s="61" t="s">
+      <c r="N14" s="64" t="s">
         <v>211</v>
       </c>
-      <c r="O14" s="62"/>
-      <c r="P14" s="63"/>
-      <c r="Q14" s="61" t="s">
+      <c r="O14" s="65"/>
+      <c r="P14" s="66"/>
+      <c r="Q14" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="R14" s="62"/>
-      <c r="S14" s="63"/>
+      <c r="R14" s="65"/>
+      <c r="S14" s="66"/>
     </row>
     <row r="15" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
@@ -5032,16 +5168,16 @@
       <c r="M15" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="N15" s="64" t="s">
+      <c r="N15" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="O15" s="65"/>
-      <c r="P15" s="66"/>
-      <c r="Q15" s="61" t="s">
+      <c r="O15" s="62"/>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="64" t="s">
         <v>219</v>
       </c>
-      <c r="R15" s="62"/>
-      <c r="S15" s="63"/>
+      <c r="R15" s="65"/>
+      <c r="S15" s="66"/>
     </row>
     <row r="16" spans="1:19" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
@@ -5083,16 +5219,16 @@
       <c r="M16" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="N16" s="64" t="s">
+      <c r="N16" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="O16" s="65"/>
-      <c r="P16" s="66"/>
-      <c r="Q16" s="61" t="s">
+      <c r="O16" s="62"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="64" t="s">
         <v>228</v>
       </c>
-      <c r="R16" s="62"/>
-      <c r="S16" s="63"/>
+      <c r="R16" s="65"/>
+      <c r="S16" s="66"/>
     </row>
     <row r="17" spans="1:19" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
@@ -5134,16 +5270,16 @@
       <c r="M17" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="N17" s="61" t="s">
+      <c r="N17" s="64" t="s">
         <v>234</v>
       </c>
-      <c r="O17" s="62"/>
-      <c r="P17" s="63"/>
-      <c r="Q17" s="61" t="s">
+      <c r="O17" s="65"/>
+      <c r="P17" s="66"/>
+      <c r="Q17" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="R17" s="62"/>
-      <c r="S17" s="63"/>
+      <c r="R17" s="65"/>
+      <c r="S17" s="66"/>
     </row>
     <row r="18" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="39" t="s">
@@ -5185,16 +5321,16 @@
       <c r="M18" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="N18" s="64" t="s">
+      <c r="N18" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="O18" s="65"/>
-      <c r="P18" s="66"/>
-      <c r="Q18" s="61" t="s">
+      <c r="O18" s="62"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="64" t="s">
         <v>239</v>
       </c>
-      <c r="R18" s="62"/>
-      <c r="S18" s="63"/>
+      <c r="R18" s="65"/>
+      <c r="S18" s="66"/>
     </row>
     <row r="19" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="41" t="s">
@@ -5236,16 +5372,16 @@
       <c r="M19" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="N19" s="61" t="s">
+      <c r="N19" s="64" t="s">
         <v>245</v>
       </c>
-      <c r="O19" s="62"/>
-      <c r="P19" s="63"/>
-      <c r="Q19" s="61" t="s">
+      <c r="O19" s="65"/>
+      <c r="P19" s="66"/>
+      <c r="Q19" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="R19" s="62"/>
-      <c r="S19" s="63"/>
+      <c r="R19" s="65"/>
+      <c r="S19" s="66"/>
     </row>
     <row r="20" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
@@ -5287,16 +5423,16 @@
       <c r="M20" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="N20" s="61" t="s">
+      <c r="N20" s="64" t="s">
         <v>250</v>
       </c>
-      <c r="O20" s="62"/>
-      <c r="P20" s="63"/>
-      <c r="Q20" s="61" t="s">
+      <c r="O20" s="65"/>
+      <c r="P20" s="66"/>
+      <c r="Q20" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="R20" s="62"/>
-      <c r="S20" s="63"/>
+      <c r="R20" s="65"/>
+      <c r="S20" s="66"/>
     </row>
     <row r="21" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
@@ -5338,16 +5474,16 @@
       <c r="M21" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="N21" s="64" t="s">
+      <c r="N21" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="O21" s="65"/>
-      <c r="P21" s="66"/>
-      <c r="Q21" s="61" t="s">
+      <c r="O21" s="62"/>
+      <c r="P21" s="63"/>
+      <c r="Q21" s="64" t="s">
         <v>255</v>
       </c>
-      <c r="R21" s="62"/>
-      <c r="S21" s="63"/>
+      <c r="R21" s="65"/>
+      <c r="S21" s="66"/>
     </row>
     <row r="22" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
@@ -5389,16 +5525,16 @@
       <c r="M22" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="N22" s="61" t="s">
+      <c r="N22" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="O22" s="62"/>
-      <c r="P22" s="63"/>
-      <c r="Q22" s="61" t="s">
+      <c r="O22" s="65"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="R22" s="62"/>
-      <c r="S22" s="63"/>
+      <c r="R22" s="65"/>
+      <c r="S22" s="66"/>
     </row>
     <row r="23" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
@@ -5440,16 +5576,16 @@
       <c r="M23" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="N23" s="64" t="s">
+      <c r="N23" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="O23" s="65"/>
-      <c r="P23" s="66"/>
-      <c r="Q23" s="61" t="s">
+      <c r="O23" s="62"/>
+      <c r="P23" s="63"/>
+      <c r="Q23" s="64" t="s">
         <v>267</v>
       </c>
-      <c r="R23" s="62"/>
-      <c r="S23" s="63"/>
+      <c r="R23" s="65"/>
+      <c r="S23" s="66"/>
     </row>
     <row r="24" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
@@ -5491,18 +5627,18 @@
       <c r="M24" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="N24" s="64" t="s">
+      <c r="N24" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="O24" s="65"/>
-      <c r="P24" s="66"/>
-      <c r="Q24" s="61" t="s">
+      <c r="O24" s="62"/>
+      <c r="P24" s="63"/>
+      <c r="Q24" s="64" t="s">
         <v>273</v>
       </c>
-      <c r="R24" s="62"/>
-      <c r="S24" s="63"/>
+      <c r="R24" s="65"/>
+      <c r="S24" s="66"/>
     </row>
-    <row r="25" spans="1:19" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>274</v>
       </c>
@@ -5542,20 +5678,170 @@
       <c r="M25" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="N25" s="61" t="s">
+      <c r="N25" s="64" t="s">
         <v>279</v>
       </c>
-      <c r="O25" s="62"/>
-      <c r="P25" s="63"/>
-      <c r="Q25" s="61" t="s">
+      <c r="O25" s="65"/>
+      <c r="P25" s="66"/>
+      <c r="Q25" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="R25" s="62"/>
-      <c r="S25" s="63"/>
+      <c r="R25" s="65"/>
+      <c r="S25" s="66"/>
     </row>
-    <row r="26" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="71" t="s">
+        <v>280</v>
+      </c>
+      <c r="B26" s="72" t="s">
+        <v>281</v>
+      </c>
+      <c r="C26" s="72" t="s">
+        <v>282</v>
+      </c>
+      <c r="D26" s="72">
+        <v>6</v>
+      </c>
+      <c r="E26" s="72" t="s">
+        <v>283</v>
+      </c>
+      <c r="F26" s="72" t="s">
+        <v>284</v>
+      </c>
+      <c r="G26" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="H26" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="I26" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="J26" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="K26" s="72" t="s">
+        <v>285</v>
+      </c>
+      <c r="L26" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="M26" s="72" t="s">
+        <v>150</v>
+      </c>
+      <c r="N26" s="61" t="s">
+        <v>136</v>
+      </c>
+      <c r="O26" s="62"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="64" t="s">
+        <v>286</v>
+      </c>
+      <c r="R26" s="65"/>
+      <c r="S26" s="66"/>
+    </row>
+    <row r="27" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="73" t="s">
+        <v>287</v>
+      </c>
+      <c r="B27" s="74" t="s">
+        <v>281</v>
+      </c>
+      <c r="C27" s="74" t="s">
+        <v>288</v>
+      </c>
+      <c r="D27" s="74">
+        <v>3</v>
+      </c>
+      <c r="E27" s="74" t="s">
+        <v>289</v>
+      </c>
+      <c r="F27" s="74" t="s">
+        <v>290</v>
+      </c>
+      <c r="G27" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="H27" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="I27" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="J27" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="K27" s="74" t="s">
+        <v>291</v>
+      </c>
+      <c r="L27" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="M27" s="74" t="s">
+        <v>150</v>
+      </c>
+      <c r="N27" s="61" t="s">
+        <v>136</v>
+      </c>
+      <c r="O27" s="62"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="64" t="s">
+        <v>292</v>
+      </c>
+      <c r="R27" s="65"/>
+      <c r="S27" s="66"/>
+    </row>
+    <row r="28" spans="1:19" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="73" t="s">
+        <v>293</v>
+      </c>
+      <c r="B28" s="74" t="s">
+        <v>281</v>
+      </c>
+      <c r="C28" s="74" t="s">
+        <v>294</v>
+      </c>
+      <c r="D28" s="74">
+        <v>74</v>
+      </c>
+      <c r="E28" s="74" t="s">
+        <v>295</v>
+      </c>
+      <c r="F28" s="74" t="s">
+        <v>296</v>
+      </c>
+      <c r="G28" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="H28" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="I28" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="J28" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="K28" s="74" t="s">
+        <v>297</v>
+      </c>
+      <c r="L28" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="M28" s="74" t="s">
+        <v>150</v>
+      </c>
+      <c r="N28" s="64" t="s">
+        <v>298</v>
+      </c>
+      <c r="O28" s="65"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="64" t="s">
+        <v>137</v>
+      </c>
+      <c r="R28" s="65"/>
+      <c r="S28" s="66"/>
+    </row>
     <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6520,13 +6806,39 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="Q25:S25"/>
+  <mergeCells count="54">
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
     <mergeCell ref="N18:P18"/>
     <mergeCell ref="Q18:S18"/>
     <mergeCell ref="N19:P19"/>
@@ -6543,32 +6855,12 @@
     <mergeCell ref="Q16:S16"/>
     <mergeCell ref="N17:P17"/>
     <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="Q25:S25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>